<commit_message>
reworked the whole filtering including toxicity moiety
</commit_message>
<xml_diff>
--- a/hp1_clean.xlsx
+++ b/hp1_clean.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>zinc_id</t>
   </si>
@@ -25,18 +25,72 @@
     <t>ROMol</t>
   </si>
   <si>
+    <t>Asphericity</t>
+  </si>
+  <si>
+    <t>Eccentricity</t>
+  </si>
+  <si>
+    <t>InertialShapeFactor</t>
+  </si>
+  <si>
+    <t>NPR1</t>
+  </si>
+  <si>
+    <t>NPR2</t>
+  </si>
+  <si>
+    <t>PMI1</t>
+  </si>
+  <si>
+    <t>PMI2</t>
+  </si>
+  <si>
+    <t>PMI3</t>
+  </si>
+  <si>
+    <t>RadiusOfGyration</t>
+  </si>
+  <si>
+    <t>SpherocityIndex</t>
+  </si>
+  <si>
     <t>molecular_weight</t>
   </si>
   <si>
     <t>formal_charge</t>
   </si>
   <si>
-    <t>esters</t>
+    <t>NumHAcceptors</t>
+  </si>
+  <si>
+    <t>NumHDonors</t>
+  </si>
+  <si>
+    <t>TPSA</t>
+  </si>
+  <si>
+    <t>NumHeteroatoms</t>
+  </si>
+  <si>
+    <t>NumRotatableBonds</t>
   </si>
   <si>
     <t>similarity</t>
   </si>
   <si>
+    <t>ZINC000257347364</t>
+  </si>
+  <si>
+    <t>NS(=O)(=O)c1ccc(NC2(O)OC(CO)C(O)C(O)C2O)cc1</t>
+  </si>
+  <si>
+    <t>ZINC000091746364</t>
+  </si>
+  <si>
+    <t>CC(O)C(N)C(=O)N1CCC2(CC1)c1nc[nH]c1CCN2S(C)(=O)=O</t>
+  </si>
+  <si>
     <t>ZINC000012652346</t>
   </si>
   <si>
@@ -46,6 +100,18 @@
     <t>Cn1[n-]c(=O)c(=O)nc1SCC1=C(C(=O)[O-])N2C(=O)C(N)C2SC1</t>
   </si>
   <si>
+    <t>ZINC000091426318</t>
+  </si>
+  <si>
+    <t>CS(=O)(=O)N1CCc2nc[nH]c2C12CCN(C(=O)CNC(N)=O)CC2</t>
+  </si>
+  <si>
+    <t>ZINC000082096551</t>
+  </si>
+  <si>
+    <t>COCC(=O)N1CCN(C(=O)c2ncccc2[O-])C2CS(=O)(=O)CC21</t>
+  </si>
+  <si>
     <t>ZINC000091894352</t>
   </si>
   <si>
@@ -58,22 +124,40 @@
     <t>O=C([O-])CCN1CCN(C(=O)c2c[nH]c(=O)cn2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
-    <t>ZINC000528542410</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)[N-]C2Cc3ccccc3NC2=O)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
     <t>ZINC000096163552</t>
   </si>
   <si>
     <t>CS(=O)(=O)N1CC2CN(Cc3nc4ncccn4n3)CC2(C(=O)[O-])C1</t>
   </si>
   <si>
-    <t>ZINC000017144342</t>
-  </si>
-  <si>
-    <t>Cn1c(N)c(S(=O)(=O)[N-]Cc2ccc3c(c2)OCO3)c(=O)n(C)c1=O</t>
+    <t>ZINC000091563350</t>
+  </si>
+  <si>
+    <t>COCc1noc(CN2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)n1</t>
+  </si>
+  <si>
+    <t>ZINC000077407345</t>
+  </si>
+  <si>
+    <t>NC(CO)C(=O)N1CCc2ccc(S(=O)(=O)N3CCOCC3)cc2C1</t>
+  </si>
+  <si>
+    <t>ZINC000077506055</t>
+  </si>
+  <si>
+    <t>NC(CO)C(=O)N1CCc2cc(S(=O)(=O)N3CCOCC3)ccc2C1</t>
+  </si>
+  <si>
+    <t>ZINC000071760227</t>
+  </si>
+  <si>
+    <t>O=C([O-])C1CN(S(=O)(=O)c2ccc(N3CCOCC3)nc2)CCN1</t>
+  </si>
+  <si>
+    <t>ZINC000077389714</t>
+  </si>
+  <si>
+    <t>COCC(=O)N1CCN(C(=O)c2cc(C)[nH]n2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
     <t>ZINC000091745422</t>
@@ -82,6 +166,12 @@
     <t>CCCS(=O)(=O)N1CCN(CCC(=O)[O-])C2CS(=O)(=O)CC21</t>
   </si>
   <si>
+    <t>ZINC000072411496</t>
+  </si>
+  <si>
+    <t>CS(=O)(=O)N1CCOC(CNC(=O)CCc2cc3n(n2)CCNC3)C1</t>
+  </si>
+  <si>
     <t>ZINC000096151859</t>
   </si>
   <si>
@@ -100,10 +190,10 @@
     <t>O=C([O-])CN1CCN(Cc2nc(C(=O)[O-])co2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
-    <t>ZINC000024345326</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)[N-]C2(C)CCS(=O)(=O)C2)c(=O)n(C)c1=O</t>
+    <t>ZINC000091603058</t>
+  </si>
+  <si>
+    <t>COCc1nc(CN2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)no1</t>
   </si>
   <si>
     <t>ZINC000009307887</t>
@@ -118,34 +208,34 @@
     <t>Cn1c([O-])c(S(=O)c2c([O-])n(C)c(=O)n(C)c2=O)c(=O)n(C)c1=O</t>
   </si>
   <si>
+    <t>ZINC000670472389</t>
+  </si>
+  <si>
+    <t>Cn1cc(S(=O)(=O)NCCN2CCCCC2CO)c(=O)n(C)c1=O</t>
+  </si>
+  <si>
+    <t>ZINC000091988472</t>
+  </si>
+  <si>
+    <t>CN1CC(NC(=O)c2ccc(S(=O)(=O)NCCO)cc2)CC1CO</t>
+  </si>
+  <si>
     <t>ZINC000077353848</t>
   </si>
   <si>
     <t>O=C([O-])CN1CCN(C(=O)CCCn2cncn2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
-    <t>ZINC000056103857</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)[N-]CC(=O)NCC(F)(F)F)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000244875028</t>
-  </si>
-  <si>
-    <t>Cc1nc(NC(=O)CN2CCN(S(N)(=O)=O)CC2)sc1C(=O)[O-]</t>
-  </si>
-  <si>
-    <t>ZINC000585138604</t>
-  </si>
-  <si>
-    <t>CS(C)(=O)=NS(=O)(=O)N1CCN(C(=O)C2(C(=O)[O-])CC2)CC1</t>
-  </si>
-  <si>
-    <t>ZINC000952987906</t>
-  </si>
-  <si>
-    <t>Cc1ccc(S(=O)(=O)N2CCN(C(=O)Cn3[n-]nnc3=N)CC2)cc1</t>
+    <t>ZINC000670448199</t>
+  </si>
+  <si>
+    <t>Cn1cc(S(=O)(=O)NCCN2CCCC(CO)C2)c(=O)n(C)c1=O</t>
+  </si>
+  <si>
+    <t>ZINC000091574424</t>
+  </si>
+  <si>
+    <t>O=C([O-])CCN1CCN(C(=O)N2CCOCC2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
     <t>ZINC000092022362</t>
@@ -154,12 +244,6 @@
     <t>CN1CCN(C(=O)N2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)CC1</t>
   </si>
   <si>
-    <t>ZINC000002898447</t>
-  </si>
-  <si>
-    <t>Cc1[nH]c(=O)[nH]c(=O)c1S(=O)(=O)[N-]c1ccc(S(N)(=O)=O)cc1</t>
-  </si>
-  <si>
     <t>ZINC000012687369</t>
   </si>
   <si>
@@ -172,16 +256,22 @@
     <t>NS(=O)(=O)c1ccc(NC(=O)CSc2n[nH]c(=O)[n-]c2=O)cc1</t>
   </si>
   <si>
-    <t>ZINC000001532061</t>
-  </si>
-  <si>
-    <t>COc1cc(OC)nc(NC(=O)[N-]S(=O)(=O)N(C)S(C)(=O)=O)n1</t>
-  </si>
-  <si>
     <t>ZINC000091288550</t>
   </si>
   <si>
     <t>Cn1nnnc1SCCNC(=O)c1cnc(Cn2cncn2)[n-]c1=O</t>
+  </si>
+  <si>
+    <t>ZINC000330730473</t>
+  </si>
+  <si>
+    <t>CN(C)CC(=O)N1CCN(S(=O)(=O)CCCN2CCOCC2)CC1</t>
+  </si>
+  <si>
+    <t>ZINC000035552524</t>
+  </si>
+  <si>
+    <t>CS(=O)(=O)N(CCCN1CCOCC1)CCC(=O)N1CCNCC1</t>
   </si>
   <si>
     <t>ZINC000006095847</t>
@@ -1215,6 +1305,310 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1219200" y="95440500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="99250500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="103060500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="106870500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="110680500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="114490500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="118300500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="122110500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="125920500"/>
           <a:ext cx="2857500" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1512,7 +1906,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1521,7 +1915,7 @@
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,524 +1937,2154 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="300" customHeight="1">
+    <row r="2" spans="1:21" ht="300" customHeight="1">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>0.5846432169582619</v>
+      </c>
+      <c r="E2">
+        <v>0.985893414103122</v>
+      </c>
+      <c r="F2">
+        <v>0.001121872241738584</v>
+      </c>
+      <c r="G2">
+        <v>0.1673743589325732</v>
+      </c>
+      <c r="H2">
+        <v>0.9594063749865595</v>
+      </c>
+      <c r="I2">
+        <v>855.1832724729431</v>
+      </c>
+      <c r="J2">
+        <v>4901.995076336246</v>
+      </c>
+      <c r="K2">
+        <v>5109.404319316639</v>
+      </c>
+      <c r="L2">
+        <v>4.043850394446073</v>
+      </c>
+      <c r="M2">
+        <v>0.192178247936826</v>
+      </c>
+      <c r="N2">
+        <v>352.4160000000002</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>112.81</v>
+      </c>
+      <c r="S2">
+        <v>9</v>
+      </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
+      <c r="U2">
+        <v>0.3979148566463944</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="300" customHeight="1">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>0.4906594722358194</v>
+      </c>
+      <c r="E3">
+        <v>0.9767682080392288</v>
+      </c>
+      <c r="F3">
+        <v>0.0009177723299327842</v>
+      </c>
+      <c r="G3">
+        <v>0.2142985482074799</v>
+      </c>
+      <c r="H3">
+        <v>0.8932374660082714</v>
+      </c>
+      <c r="I3">
+        <v>973.2669387338036</v>
+      </c>
+      <c r="J3">
+        <v>4056.763339630809</v>
+      </c>
+      <c r="K3">
+        <v>4541.640374490566</v>
+      </c>
+      <c r="L3">
+        <v>3.728355380948158</v>
+      </c>
+      <c r="M3">
+        <v>0.154886579713828</v>
+      </c>
+      <c r="N3">
+        <v>364.4490000000002</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>131.57</v>
+      </c>
+      <c r="S3">
+        <v>11</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>0.314359637774903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="300" customHeight="1">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>0.3449552659626504</v>
+      </c>
+      <c r="E4">
+        <v>0.9510808943401239</v>
+      </c>
+      <c r="F4">
+        <v>0.0005577448750631422</v>
+      </c>
+      <c r="G4">
+        <v>0.3089419563950321</v>
+      </c>
+      <c r="H4">
+        <v>0.7611068055412593</v>
+      </c>
+      <c r="I4">
+        <v>1364.614610676781</v>
+      </c>
+      <c r="J4">
+        <v>3361.853078314471</v>
+      </c>
+      <c r="K4">
+        <v>4417.058228672252</v>
+      </c>
+      <c r="L4">
+        <v>3.633519713547636</v>
+      </c>
+      <c r="M4">
+        <v>0.1086263544986856</v>
+      </c>
+      <c r="N4">
+        <v>363.4170000000001</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>117.86</v>
+      </c>
+      <c r="S4">
+        <v>11</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0.308381317978247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="300" customHeight="1">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>0.4309271650985923</v>
+      </c>
+      <c r="E5">
+        <v>0.9685243186049406</v>
+      </c>
+      <c r="F5">
+        <v>0.0006926963921350542</v>
+      </c>
+      <c r="G5">
+        <v>0.2489189512086924</v>
+      </c>
+      <c r="H5">
+        <v>0.8237015423531667</v>
+      </c>
+      <c r="I5">
+        <v>1189.12347704645</v>
+      </c>
+      <c r="J5">
+        <v>3934.946846495138</v>
+      </c>
+      <c r="K5">
+        <v>4777.151242492158</v>
+      </c>
+      <c r="L5">
+        <v>3.717135664444417</v>
+      </c>
+      <c r="M5">
+        <v>0.1090918048168907</v>
+      </c>
+      <c r="N5">
+        <v>369.3840000000001</v>
+      </c>
+      <c r="O5">
+        <v>-2</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>152.52</v>
+      </c>
+      <c r="S5">
+        <v>12</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>0.3069498069498069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="300" customHeight="1">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>0.7722535688004022</v>
+      </c>
+      <c r="E6">
+        <v>0.9965611605726561</v>
+      </c>
+      <c r="F6">
+        <v>0.001372657827770624</v>
+      </c>
+      <c r="G6">
+        <v>0.08286044435121516</v>
+      </c>
+      <c r="H6">
+        <v>0.9515155028443129</v>
+      </c>
+      <c r="I6">
+        <v>693.192056748548</v>
+      </c>
+      <c r="J6">
+        <v>7960.167165518045</v>
+      </c>
+      <c r="K6">
+        <v>8365.777690140787</v>
+      </c>
+      <c r="L6">
+        <v>4.971554384167305</v>
+      </c>
+      <c r="M6">
+        <v>0.05094549195576247</v>
+      </c>
+      <c r="N6">
+        <v>360.4170000000001</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>133.8</v>
+      </c>
+      <c r="S6">
+        <v>11</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>0.3051398828887443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="300" customHeight="1">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>0.5708675857338262</v>
+      </c>
+      <c r="E7">
+        <v>0.9850930317828652</v>
+      </c>
+      <c r="F7">
+        <v>0.001063572838338249</v>
+      </c>
+      <c r="G7">
+        <v>0.1720224367134792</v>
+      </c>
+      <c r="H7">
+        <v>0.8992785886654669</v>
+      </c>
+      <c r="I7">
+        <v>845.5260949222062</v>
+      </c>
+      <c r="J7">
+        <v>4420.141510888651</v>
+      </c>
+      <c r="K7">
+        <v>4915.208219788886</v>
+      </c>
+      <c r="L7">
+        <v>3.914077247657001</v>
+      </c>
+      <c r="M7">
+        <v>0.1225464180700887</v>
+      </c>
+      <c r="N7">
+        <v>352.4340000000001</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>108.9</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>0.2851959361393324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="300" customHeight="1">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>0.5370800285465821</v>
+      </c>
+      <c r="E8">
+        <v>0.9819813035158284</v>
+      </c>
+      <c r="F8">
+        <v>0.0008907438088225321</v>
+      </c>
+      <c r="G8">
+        <v>0.1889780927656821</v>
+      </c>
+      <c r="H8">
+        <v>0.8704297112809343</v>
+      </c>
+      <c r="I8">
+        <v>977.1942310006613</v>
+      </c>
+      <c r="J8">
+        <v>4500.939129542125</v>
+      </c>
+      <c r="K8">
+        <v>5170.939216813373</v>
+      </c>
+      <c r="L8">
+        <v>3.955972979567874</v>
+      </c>
+      <c r="M8">
+        <v>0.08898898629685369</v>
+      </c>
+      <c r="N8">
+        <v>360.3920000000001</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>369.3840000000001</v>
-      </c>
-      <c r="E2">
-        <v>-2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0.308381317978247</v>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>119.71</v>
+      </c>
+      <c r="S8">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <v>0.2759365994236311</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="300" customHeight="1">
-      <c r="A3" t="s">
+    <row r="9" spans="1:21" ht="300" customHeight="1">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>0.498885079185205</v>
+      </c>
+      <c r="E9">
+        <v>0.9777534653167165</v>
+      </c>
+      <c r="F9">
+        <v>0.0007580775527358738</v>
+      </c>
+      <c r="G9">
+        <v>0.2097573861897419</v>
+      </c>
+      <c r="H9">
+        <v>0.8946863957121091</v>
+      </c>
+      <c r="I9">
+        <v>1180.204310869276</v>
+      </c>
+      <c r="J9">
+        <v>5033.971676879928</v>
+      </c>
+      <c r="K9">
+        <v>5626.52086921835</v>
+      </c>
+      <c r="L9">
+        <v>4.099302010316602</v>
+      </c>
+      <c r="M9">
+        <v>0.1718575465412039</v>
+      </c>
+      <c r="N9">
+        <v>374.4880000000001</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>116.83</v>
+      </c>
+      <c r="S9">
+        <v>10</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="U9">
+        <v>0.2732778198334595</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="300" customHeight="1">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>0.4701098577918231</v>
+      </c>
+      <c r="E10">
+        <v>0.9741853374449321</v>
+      </c>
+      <c r="F10">
+        <v>0.0006738366626951883</v>
+      </c>
+      <c r="G10">
+        <v>0.2257497027845301</v>
+      </c>
+      <c r="H10">
+        <v>0.8311971174795549</v>
+      </c>
+      <c r="I10">
+        <v>1233.529078330291</v>
+      </c>
+      <c r="J10">
+        <v>4541.781457909459</v>
+      </c>
+      <c r="K10">
+        <v>5464.144860946506</v>
+      </c>
+      <c r="L10">
+        <v>4.017065896801048</v>
+      </c>
+      <c r="M10">
+        <v>0.08913781512818016</v>
+      </c>
+      <c r="N10">
+        <v>370.4310000000002</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>119.39</v>
+      </c>
+      <c r="S10">
+        <v>10</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>0.2693156732891832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="300" customHeight="1">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>0.5924543544911338</v>
+      </c>
+      <c r="E11">
+        <v>0.9866363473260849</v>
+      </c>
+      <c r="F11">
+        <v>0.001087280961573521</v>
+      </c>
+      <c r="G11">
+        <v>0.1629377738127083</v>
+      </c>
+      <c r="H11">
+        <v>0.9494030519616842</v>
+      </c>
+      <c r="I11">
+        <v>873.1901739433578</v>
+      </c>
+      <c r="J11">
+        <v>5087.88966908126</v>
+      </c>
+      <c r="K11">
+        <v>5359.040776800237</v>
+      </c>
+      <c r="L11">
+        <v>4.031455303526324</v>
+      </c>
+      <c r="M11">
+        <v>0.1759729182455492</v>
+      </c>
+      <c r="N11">
+        <v>372.4470000000001</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>110.48</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>0.2663438256658596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="300" customHeight="1">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
+        <v>0.6657056224767195</v>
+      </c>
+      <c r="E12">
+        <v>0.9918386362210143</v>
+      </c>
+      <c r="F12">
+        <v>0.001174263379651534</v>
+      </c>
+      <c r="G12">
+        <v>0.127499489015598</v>
+      </c>
+      <c r="H12">
+        <v>0.9140280285056589</v>
+      </c>
+      <c r="I12">
+        <v>778.3841720218675</v>
+      </c>
+      <c r="J12">
+        <v>5580.139619901677</v>
+      </c>
+      <c r="K12">
+        <v>6104.998365339658</v>
+      </c>
+      <c r="L12">
+        <v>4.230134954038514</v>
+      </c>
+      <c r="M12">
+        <v>0.06960301393463061</v>
+      </c>
+      <c r="N12">
+        <v>370.4350000000002</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>369.3840000000001</v>
-      </c>
-      <c r="E3">
-        <v>-2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.3069498069498069</v>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>102.44</v>
+      </c>
+      <c r="S12">
+        <v>11</v>
+      </c>
+      <c r="T12">
+        <v>4</v>
+      </c>
+      <c r="U12">
+        <v>0.2637277648878577</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="300" customHeight="1">
-      <c r="A4" t="s">
+    <row r="13" spans="1:21" ht="300" customHeight="1">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>0.4663352874565803</v>
+      </c>
+      <c r="E13">
+        <v>0.9730357331053255</v>
+      </c>
+      <c r="F13">
+        <v>0.0009242504873416692</v>
+      </c>
+      <c r="G13">
+        <v>0.2306544213757487</v>
+      </c>
+      <c r="H13">
+        <v>0.9398661374015223</v>
+      </c>
+      <c r="I13">
+        <v>1016.895473979967</v>
+      </c>
+      <c r="J13">
+        <v>4143.625843242259</v>
+      </c>
+      <c r="K13">
+        <v>4408.740434779652</v>
+      </c>
+      <c r="L13">
+        <v>3.706598443578781</v>
+      </c>
+      <c r="M13">
+        <v>0.2293665451897019</v>
+      </c>
+      <c r="N13">
+        <v>374.4630000000002</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>8</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>102.64</v>
+      </c>
+      <c r="S13">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="T13">
+        <v>6</v>
+      </c>
+      <c r="U13">
+        <v>0.2636080870917574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="300" customHeight="1">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>0.4984411504578892</v>
+      </c>
+      <c r="E14">
+        <v>0.977623809770786</v>
+      </c>
+      <c r="F14">
+        <v>0.0009057621926329796</v>
+      </c>
+      <c r="G14">
+        <v>0.2103608484705597</v>
+      </c>
+      <c r="H14">
+        <v>0.9058309327648238</v>
+      </c>
+      <c r="I14">
+        <v>1000.075892030384</v>
+      </c>
+      <c r="J14">
+        <v>4306.408177661814</v>
+      </c>
+      <c r="K14">
+        <v>4754.09706369551</v>
+      </c>
+      <c r="L14">
+        <v>3.879331833145499</v>
+      </c>
+      <c r="M14">
+        <v>0.1696517532485974</v>
+      </c>
+      <c r="N14">
+        <v>357.4400000000001</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>7</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>104.53</v>
+      </c>
+      <c r="S14">
         <v>11</v>
       </c>
-      <c r="D4">
-        <v>356.3800000000002</v>
-      </c>
-      <c r="E4">
-        <v>-1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0.2759365994236311</v>
+      <c r="T14">
+        <v>5</v>
+      </c>
+      <c r="U14">
+        <v>0.2626339969372128</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="300" customHeight="1">
-      <c r="A5" t="s">
+    <row r="15" spans="1:21" ht="300" customHeight="1">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>0.7762901422904512</v>
+      </c>
+      <c r="E15">
+        <v>0.9966588676495182</v>
+      </c>
+      <c r="F15">
+        <v>0.001866376355933924</v>
+      </c>
+      <c r="G15">
+        <v>0.08167681149249317</v>
+      </c>
+      <c r="H15">
+        <v>0.9739419885855243</v>
+      </c>
+      <c r="I15">
+        <v>521.8357945271812</v>
+      </c>
+      <c r="J15">
+        <v>6222.546915701055</v>
+      </c>
+      <c r="K15">
+        <v>6389.032394771465</v>
+      </c>
+      <c r="L15">
+        <v>4.432378406814022</v>
+      </c>
+      <c r="M15">
+        <v>0.08605198427876341</v>
+      </c>
+      <c r="N15">
+        <v>351.3880000000001</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>7</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>105.47</v>
+      </c>
+      <c r="S15">
+        <v>10</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <v>0.2620997766195086</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="300" customHeight="1">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>0.4521946896802228</v>
+      </c>
+      <c r="E16">
+        <v>0.9717963302796065</v>
+      </c>
+      <c r="F16">
+        <v>0.0006609068887957628</v>
+      </c>
+      <c r="G16">
+        <v>0.2358217387245924</v>
+      </c>
+      <c r="H16">
+        <v>0.8509425515174648</v>
+      </c>
+      <c r="I16">
+        <v>1287.53772421402</v>
+      </c>
+      <c r="J16">
+        <v>4645.969630039931</v>
+      </c>
+      <c r="K16">
+        <v>5459.792346445583</v>
+      </c>
+      <c r="L16">
+        <v>4.01015885182064</v>
+      </c>
+      <c r="M16">
+        <v>0.1218556277968444</v>
+      </c>
+      <c r="N16">
+        <v>373.3910000000001</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>9</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>148.93</v>
+      </c>
+      <c r="S16">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="U16">
+        <v>0.2596078431372549</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="300" customHeight="1">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>0.6195773890165506</v>
+      </c>
+      <c r="E17">
+        <v>0.9889088623450888</v>
+      </c>
+      <c r="F17">
+        <v>0.001050461832639103</v>
+      </c>
+      <c r="G17">
+        <v>0.1485236074681138</v>
+      </c>
+      <c r="H17">
+        <v>0.906372970627521</v>
+      </c>
+      <c r="I17">
+        <v>862.8328440552818</v>
+      </c>
+      <c r="J17">
+        <v>5265.481907913356</v>
+      </c>
+      <c r="K17">
+        <v>5809.398645535332</v>
+      </c>
+      <c r="L17">
+        <v>4.139967158683688</v>
+      </c>
+      <c r="M17">
+        <v>0.08812684507888002</v>
+      </c>
+      <c r="N17">
+        <v>366.3990000000001</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>8</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>120.13</v>
+      </c>
+      <c r="S17">
+        <v>10</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <v>0.2589147286821705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="300" customHeight="1">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>0.4379754417308929</v>
+      </c>
+      <c r="E18">
+        <v>0.9696875734366118</v>
+      </c>
+      <c r="F18">
+        <v>0.0006084950156751938</v>
+      </c>
+      <c r="G18">
+        <v>0.2443481326358271</v>
+      </c>
+      <c r="H18">
+        <v>0.8404205452837877</v>
+      </c>
+      <c r="I18">
+        <v>1381.146145217388</v>
+      </c>
+      <c r="J18">
+        <v>4750.368189676956</v>
+      </c>
+      <c r="K18">
+        <v>5652.37037139886</v>
+      </c>
+      <c r="L18">
+        <v>4.101493545933755</v>
+      </c>
+      <c r="M18">
+        <v>0.1205180511638987</v>
+      </c>
+      <c r="N18">
+        <v>371.4150000000001</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>6</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>114.04</v>
+      </c>
+      <c r="S18">
+        <v>10</v>
+      </c>
+      <c r="T18">
+        <v>7</v>
+      </c>
+      <c r="U18">
+        <v>0.2556221889055472</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="300" customHeight="1">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19">
+        <v>0.6670259344653984</v>
+      </c>
+      <c r="E19">
+        <v>0.9918150557458995</v>
+      </c>
+      <c r="F19">
+        <v>0.001170080156105049</v>
+      </c>
+      <c r="G19">
+        <v>0.1276827913062611</v>
+      </c>
+      <c r="H19">
+        <v>0.9503417957563013</v>
+      </c>
+      <c r="I19">
+        <v>812.2023015241872</v>
+      </c>
+      <c r="J19">
+        <v>6045.213970115071</v>
+      </c>
+      <c r="K19">
+        <v>6361.094500010038</v>
+      </c>
+      <c r="L19">
+        <v>4.356373348898332</v>
+      </c>
+      <c r="M19">
+        <v>0.1148041413675377</v>
+      </c>
+      <c r="N19">
+        <v>366.4030000000001</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>9</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>120.05</v>
+      </c>
+      <c r="S19">
+        <v>11</v>
+      </c>
+      <c r="T19">
+        <v>4</v>
+      </c>
+      <c r="U19">
+        <v>0.2548262548262548</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="300" customHeight="1">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20">
+        <v>0.2267249140963487</v>
+      </c>
+      <c r="E20">
+        <v>0.9113676632772407</v>
+      </c>
+      <c r="F20">
+        <v>0.0004094361628664221</v>
+      </c>
+      <c r="G20">
+        <v>0.4115932243521288</v>
+      </c>
+      <c r="H20">
+        <v>0.7314961632279725</v>
+      </c>
+      <c r="I20">
+        <v>1786.593929824958</v>
+      </c>
+      <c r="J20">
+        <v>3175.18979320045</v>
+      </c>
+      <c r="K20">
+        <v>4340.678670396382</v>
+      </c>
+      <c r="L20">
+        <v>3.730349773446264</v>
+      </c>
+      <c r="M20">
+        <v>0.2102725624910737</v>
+      </c>
+      <c r="N20">
+        <v>361.4640000000001</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>6</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>87.22999999999999</v>
+      </c>
+      <c r="S20">
+        <v>9</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>0.2534142640364188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="300" customHeight="1">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21">
+        <v>0.7198834740868743</v>
+      </c>
+      <c r="E21">
+        <v>0.9944361521023837</v>
+      </c>
+      <c r="F21">
+        <v>0.001346891739418987</v>
+      </c>
+      <c r="G21">
+        <v>0.1053410622302858</v>
+      </c>
+      <c r="H21">
+        <v>0.9771329643189174</v>
+      </c>
+      <c r="I21">
+        <v>725.472534815921</v>
+      </c>
+      <c r="J21">
+        <v>6729.409343974076</v>
+      </c>
+      <c r="K21">
+        <v>6886.892152558397</v>
+      </c>
+      <c r="L21">
+        <v>4.537642506676654</v>
+      </c>
+      <c r="M21">
+        <v>0.09357795293439249</v>
+      </c>
+      <c r="N21">
+        <v>362.379</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>12</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>138.3</v>
+      </c>
+      <c r="S21">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>369.3790000000001</v>
-      </c>
-      <c r="E5">
-        <v>-1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.2732778198334595</v>
+      <c r="T21">
+        <v>7</v>
+      </c>
+      <c r="U21">
+        <v>0.2479806138933764</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="300" customHeight="1">
-      <c r="A6" t="s">
+    <row r="22" spans="1:21" ht="300" customHeight="1">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>0.611904032504493</v>
+      </c>
+      <c r="E22">
+        <v>0.9883260469454799</v>
+      </c>
+      <c r="F22">
+        <v>0.0009119892525715434</v>
+      </c>
+      <c r="G22">
+        <v>0.1523536180375151</v>
+      </c>
+      <c r="H22">
+        <v>0.9177898546827249</v>
+      </c>
+      <c r="I22">
+        <v>1006.360384286137</v>
+      </c>
+      <c r="J22">
+        <v>6062.391971715388</v>
+      </c>
+      <c r="K22">
+        <v>6605.424913757763</v>
+      </c>
+      <c r="L22">
+        <v>4.443575476855749</v>
+      </c>
+      <c r="M22">
+        <v>0.1139950280633552</v>
+      </c>
+      <c r="N22">
+        <v>371.4630000000002</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>7</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>105.56</v>
+      </c>
+      <c r="S22">
+        <v>10</v>
+      </c>
+      <c r="T22">
+        <v>6</v>
+      </c>
+      <c r="U22">
+        <v>0.246422893481717</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="300" customHeight="1">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>0.2655372629737516</v>
+      </c>
+      <c r="E23">
+        <v>0.9213422831385801</v>
+      </c>
+      <c r="F23">
+        <v>0.0003645423499363801</v>
+      </c>
+      <c r="G23">
+        <v>0.3887523598654915</v>
+      </c>
+      <c r="H23">
+        <v>0.6682841852922914</v>
+      </c>
+      <c r="I23">
+        <v>1833.214125626063</v>
+      </c>
+      <c r="J23">
+        <v>3151.384106926635</v>
+      </c>
+      <c r="K23">
+        <v>4715.634719903323</v>
+      </c>
+      <c r="L23">
+        <v>3.731877710580078</v>
+      </c>
+      <c r="M23">
+        <v>0.08365118004526625</v>
+      </c>
+      <c r="N23">
+        <v>368.4150000000001</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>7</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>109.77</v>
+      </c>
+      <c r="S23">
+        <v>10</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="U23">
+        <v>0.2431192660550459</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="300" customHeight="1">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24">
+        <v>0.4133532567733383</v>
+      </c>
+      <c r="E24">
+        <v>0.9655618938301685</v>
+      </c>
+      <c r="F24">
+        <v>0.0006018782602284369</v>
+      </c>
+      <c r="G24">
+        <v>0.2601734597976865</v>
+      </c>
+      <c r="H24">
+        <v>0.8101135269594429</v>
+      </c>
+      <c r="I24">
+        <v>1345.975723814933</v>
+      </c>
+      <c r="J24">
+        <v>4191.023718058734</v>
+      </c>
+      <c r="K24">
+        <v>5173.37827179443</v>
+      </c>
+      <c r="L24">
+        <v>3.932641446347698</v>
+      </c>
+      <c r="M24">
+        <v>0.1026332091942189</v>
+      </c>
+      <c r="N24">
+        <v>367.4310000000002</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>6</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>125.7</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="T24">
+        <v>4</v>
+      </c>
+      <c r="U24">
+        <v>0.239558707643814</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="300" customHeight="1">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>0.706257657528879</v>
+      </c>
+      <c r="E25">
+        <v>0.9938643232679153</v>
+      </c>
+      <c r="F25">
+        <v>0.001520157341274223</v>
+      </c>
+      <c r="G25">
+        <v>0.1106060890512307</v>
+      </c>
+      <c r="H25">
+        <v>0.9594623052163809</v>
+      </c>
+      <c r="I25">
+        <v>631.1598669201851</v>
+      </c>
+      <c r="J25">
+        <v>5475.052106713712</v>
+      </c>
+      <c r="K25">
+        <v>5706.375411464404</v>
+      </c>
+      <c r="L25">
+        <v>4.228754146039635</v>
+      </c>
+      <c r="M25">
+        <v>0.1093704751098669</v>
+      </c>
+      <c r="N25">
+        <v>351.4540000000001</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>7</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>104.61</v>
+      </c>
+      <c r="S25">
+        <v>11</v>
+      </c>
+      <c r="T25">
+        <v>6</v>
+      </c>
+      <c r="U25">
+        <v>0.237347294938918</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="300" customHeight="1">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>0.6795966306215329</v>
+      </c>
+      <c r="E26">
+        <v>0.9925873942601608</v>
+      </c>
+      <c r="F26">
+        <v>0.001154963379423137</v>
+      </c>
+      <c r="G26">
+        <v>0.1215329780587316</v>
+      </c>
+      <c r="H26">
+        <v>0.9289589962844592</v>
+      </c>
+      <c r="I26">
+        <v>804.3190051172368</v>
+      </c>
+      <c r="J26">
+        <v>6147.955786331048</v>
+      </c>
+      <c r="K26">
+        <v>6618.113190055662</v>
+      </c>
+      <c r="L26">
+        <v>4.426705183873509</v>
+      </c>
+      <c r="M26">
+        <v>0.07879367654337684</v>
+      </c>
+      <c r="N26">
+        <v>373.4750000000001</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>6</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>98.22999999999999</v>
+      </c>
+      <c r="S26">
+        <v>9</v>
+      </c>
+      <c r="T26">
+        <v>6</v>
+      </c>
+      <c r="U26">
+        <v>0.2339373970345964</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="300" customHeight="1">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27">
+        <v>0.4143800737108312</v>
+      </c>
+      <c r="E27">
+        <v>0.9658702073489382</v>
+      </c>
+      <c r="F27">
+        <v>0.0006543762115600864</v>
+      </c>
+      <c r="G27">
+        <v>0.2590265286717156</v>
+      </c>
+      <c r="H27">
+        <v>0.8688566129982944</v>
+      </c>
+      <c r="I27">
+        <v>1327.763139382572</v>
+      </c>
+      <c r="J27">
+        <v>4453.736032613155</v>
+      </c>
+      <c r="K27">
+        <v>5125.973568002178</v>
+      </c>
+      <c r="L27">
+        <v>4.03933677084367</v>
+      </c>
+      <c r="M27">
+        <v>0.194150382843434</v>
+      </c>
+      <c r="N27">
+        <v>353.4040000000001</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>103.78</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>0.232355273592387</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="300" customHeight="1">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28">
+        <v>0.2407922799886219</v>
+      </c>
+      <c r="E28">
+        <v>0.9169573768512359</v>
+      </c>
+      <c r="F28">
+        <v>0.0004200203156350914</v>
+      </c>
+      <c r="G28">
+        <v>0.3989851739577555</v>
+      </c>
+      <c r="H28">
+        <v>0.7249629141317616</v>
+      </c>
+      <c r="I28">
+        <v>1726.018688014131</v>
+      </c>
+      <c r="J28">
+        <v>3136.205602569813</v>
+      </c>
+      <c r="K28">
+        <v>4326.022119801579</v>
+      </c>
+      <c r="L28">
+        <v>3.707356174106399</v>
+      </c>
+      <c r="M28">
+        <v>0.1806839846097422</v>
+      </c>
+      <c r="N28">
+        <v>357.4360000000001</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>97.63</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="T28">
+        <v>4</v>
+      </c>
+      <c r="U28">
+        <v>0.223717409587889</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="300" customHeight="1">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29">
+        <v>0.235197908468129</v>
+      </c>
+      <c r="E29">
+        <v>0.9183381964617253</v>
+      </c>
+      <c r="F29">
+        <v>0.0005593956038327794</v>
+      </c>
+      <c r="G29">
+        <v>0.3957966105456509</v>
+      </c>
+      <c r="H29">
+        <v>0.8364846251807048</v>
+      </c>
+      <c r="I29">
+        <v>1495.336429978016</v>
+      </c>
+      <c r="J29">
+        <v>3160.274494076154</v>
+      </c>
+      <c r="K29">
+        <v>3778.042535322684</v>
+      </c>
+      <c r="L29">
+        <v>3.450183862249772</v>
+      </c>
+      <c r="M29">
+        <v>0.326678245529735</v>
+      </c>
+      <c r="N29">
+        <v>373.3950000000002</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>10</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>153.61</v>
+      </c>
+      <c r="S29">
+        <v>13</v>
+      </c>
+      <c r="T29">
+        <v>4</v>
+      </c>
+      <c r="U29">
+        <v>0.2131147540983606</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="300" customHeight="1">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30">
+        <v>0.5848817959131735</v>
+      </c>
+      <c r="E30">
+        <v>0.9862972090738625</v>
+      </c>
+      <c r="F30">
+        <v>0.0009341481804297294</v>
+      </c>
+      <c r="G30">
+        <v>0.1649782269668014</v>
+      </c>
+      <c r="H30">
+        <v>0.8875386184907657</v>
+      </c>
+      <c r="I30">
+        <v>950.1047447124263</v>
+      </c>
+      <c r="J30">
+        <v>5111.308734777933</v>
+      </c>
+      <c r="K30">
+        <v>5758.970514961444</v>
+      </c>
+      <c r="L30">
+        <v>4.192504361023125</v>
+      </c>
+      <c r="M30">
+        <v>0.07516633597461307</v>
+      </c>
+      <c r="N30">
+        <v>360.4360000000001</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>8</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30">
+        <v>113.64</v>
+      </c>
+      <c r="S30">
+        <v>10</v>
+      </c>
+      <c r="T30">
+        <v>6</v>
+      </c>
+      <c r="U30">
+        <v>0.2097053726169844</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="300" customHeight="1">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31">
+        <v>0.2813297056408623</v>
+      </c>
+      <c r="E31">
+        <v>0.9327933965186915</v>
+      </c>
+      <c r="F31">
+        <v>0.0005124871549688345</v>
+      </c>
+      <c r="G31">
+        <v>0.3604115417285124</v>
+      </c>
+      <c r="H31">
+        <v>0.7405292505034669</v>
+      </c>
+      <c r="I31">
+        <v>1444.971338937266</v>
+      </c>
+      <c r="J31">
+        <v>2968.949155985236</v>
+      </c>
+      <c r="K31">
+        <v>4009.226042005395</v>
+      </c>
+      <c r="L31">
+        <v>3.549668295417375</v>
+      </c>
+      <c r="M31">
+        <v>0.1500774932676833</v>
+      </c>
+      <c r="N31">
+        <v>361.4640000000001</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>87.22999999999999</v>
+      </c>
+      <c r="S31">
+        <v>9</v>
+      </c>
+      <c r="T31">
+        <v>5</v>
+      </c>
+      <c r="U31">
+        <v>0.2081563296516568</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="300" customHeight="1">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32">
+        <v>0.360393832452292</v>
+      </c>
+      <c r="E32">
+        <v>0.9551647918592746</v>
+      </c>
+      <c r="F32">
+        <v>0.0008743382020202426</v>
+      </c>
+      <c r="G32">
+        <v>0.2960746871862378</v>
+      </c>
+      <c r="H32">
+        <v>0.8942044442696888</v>
+      </c>
+      <c r="I32">
+        <v>1022.721462019552</v>
+      </c>
+      <c r="J32">
+        <v>3088.822233602907</v>
+      </c>
+      <c r="K32">
+        <v>3454.268487924591</v>
+      </c>
+      <c r="L32">
+        <v>3.354023763081078</v>
+      </c>
+      <c r="M32">
+        <v>0.2774593735321926</v>
+      </c>
+      <c r="N32">
+        <v>350.3860000000001</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>12</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>155.48</v>
+      </c>
+      <c r="S32">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>363.3750000000002</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0.2707903780068728</v>
+      <c r="T32">
+        <v>7</v>
+      </c>
+      <c r="U32">
+        <v>0.186536901865369</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="300" customHeight="1">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>365.3950000000002</v>
-      </c>
-      <c r="E7">
-        <v>-1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0.2693156732891832</v>
+    <row r="33" spans="1:21" ht="300" customHeight="1">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33">
+        <v>0.4390340502597004</v>
+      </c>
+      <c r="E33">
+        <v>0.9695900877354237</v>
+      </c>
+      <c r="F33">
+        <v>0.0008423005632410761</v>
+      </c>
+      <c r="G33">
+        <v>0.2447346762623012</v>
+      </c>
+      <c r="H33">
+        <v>0.8997335592361099</v>
+      </c>
+      <c r="I33">
+        <v>1068.185869155825</v>
+      </c>
+      <c r="J33">
+        <v>3927.039227376266</v>
+      </c>
+      <c r="K33">
+        <v>4364.669059038315</v>
+      </c>
+      <c r="L33">
+        <v>3.799197437509039</v>
+      </c>
+      <c r="M33">
+        <v>0.2158601450336576</v>
+      </c>
+      <c r="N33">
+        <v>350.4410000000002</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>6</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33">
+        <v>116.41</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <v>6</v>
+      </c>
+      <c r="U33">
+        <v>0.1787487586891758</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="300" customHeight="1">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>367.3630000000002</v>
-      </c>
-      <c r="E8">
-        <v>-1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0.2597669636737491</v>
+    <row r="34" spans="1:21" ht="300" customHeight="1">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34">
+        <v>0.7192041818456747</v>
+      </c>
+      <c r="E34">
+        <v>0.9944885824345713</v>
+      </c>
+      <c r="F34">
+        <v>0.001451229349131963</v>
+      </c>
+      <c r="G34">
+        <v>0.1048449302888662</v>
+      </c>
+      <c r="H34">
+        <v>0.9524863662367077</v>
+      </c>
+      <c r="I34">
+        <v>656.3306942534116</v>
+      </c>
+      <c r="J34">
+        <v>5962.577649645631</v>
+      </c>
+      <c r="K34">
+        <v>6260.013645343704</v>
+      </c>
+      <c r="L34">
+        <v>4.376203274249526</v>
+      </c>
+      <c r="M34">
+        <v>0.08898260413669914</v>
+      </c>
+      <c r="N34">
+        <v>352.3720000000001</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>6</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>107.96</v>
+      </c>
+      <c r="S34">
+        <v>10</v>
+      </c>
+      <c r="T34">
+        <v>3</v>
+      </c>
+      <c r="U34">
+        <v>0.1492693110647182</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="300" customHeight="1">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9">
-        <v>353.4420000000001</v>
-      </c>
-      <c r="E9">
-        <v>-1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0.2596078431372549</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="300" customHeight="1">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10">
-        <v>371.3950000000002</v>
-      </c>
-      <c r="E10">
-        <v>-1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0.2556221889055472</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="300" customHeight="1">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>355.3960000000002</v>
-      </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0.2548262548262548</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="300" customHeight="1">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12">
-        <v>357.3440000000001</v>
-      </c>
-      <c r="E12">
-        <v>-2</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0.2534142640364188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="300" customHeight="1">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13">
-        <v>350.3980000000001</v>
-      </c>
-      <c r="E13">
-        <v>-1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0.2529940119760479</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="300" customHeight="1">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14">
-        <v>357.4300000000001</v>
-      </c>
-      <c r="E14">
-        <v>-1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0.246422893481717</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="300" customHeight="1">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15">
-        <v>356.3160000000001</v>
-      </c>
-      <c r="E15">
-        <v>-2</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0.2431192660550459</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="300" customHeight="1">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16">
-        <v>370.4110000000001</v>
-      </c>
-      <c r="E16">
-        <v>-1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0.2339373970345964</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="300" customHeight="1">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17">
-        <v>357.2900000000001</v>
-      </c>
-      <c r="E17">
-        <v>-1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0.2268370607028754</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="300" customHeight="1">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18">
-        <v>362.4130000000001</v>
-      </c>
-      <c r="E18">
-        <v>-1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0.2195121951219512</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="300" customHeight="1">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19">
-        <v>352.4140000000002</v>
-      </c>
-      <c r="E19">
-        <v>-1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0.2176211453744493</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="300" customHeight="1">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20">
-        <v>364.4110000000001</v>
-      </c>
-      <c r="E20">
-        <v>-1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0.2173553719008264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="300" customHeight="1">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21">
-        <v>373.4550000000001</v>
-      </c>
-      <c r="E21">
-        <v>-1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0.2131147540983606</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="300" customHeight="1">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22">
-        <v>359.3650000000001</v>
-      </c>
-      <c r="E22">
-        <v>-1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0.2101167315175097</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="300" customHeight="1">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23">
-        <v>360.3970000000001</v>
-      </c>
-      <c r="E23">
-        <v>-1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0.2097053726169844</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="300" customHeight="1">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24">
-        <v>356.3650000000001</v>
-      </c>
-      <c r="E24">
-        <v>-1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0.2081563296516568</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="300" customHeight="1">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25">
-        <v>368.3730000000001</v>
-      </c>
-      <c r="E25">
-        <v>-1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0.1998284734133791</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="300" customHeight="1">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26">
-        <v>361.371</v>
-      </c>
-      <c r="E26">
-        <v>-1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0.186536901865369</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="300" customHeight="1">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27">
-        <v>366.3750000000001</v>
-      </c>
-      <c r="E27">
-        <v>-1</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
+    <row r="35" spans="1:21" ht="300" customHeight="1">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35">
+        <v>0.5207746956644161</v>
+      </c>
+      <c r="E35">
+        <v>0.9802838849018404</v>
+      </c>
+      <c r="F35">
+        <v>0.0008912360400703853</v>
+      </c>
+      <c r="G35">
+        <v>0.1975942939503953</v>
+      </c>
+      <c r="H35">
+        <v>0.8800692462864887</v>
+      </c>
+      <c r="I35">
+        <v>987.4704418562173</v>
+      </c>
+      <c r="J35">
+        <v>4398.114693093084</v>
+      </c>
+      <c r="K35">
+        <v>4997.46436050484</v>
+      </c>
+      <c r="L35">
+        <v>3.883289484747549</v>
+      </c>
+      <c r="M35">
+        <v>0.104936010932161</v>
+      </c>
+      <c r="N35">
+        <v>372.491</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>6</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>81.24000000000001</v>
+      </c>
+      <c r="S35">
+        <v>9</v>
+      </c>
+      <c r="T35">
+        <v>5</v>
+      </c>
+      <c r="U35">
         <v>0.1444788441692466</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed dictionary of 3D descriptor addition
</commit_message>
<xml_diff>
--- a/hp1_clean.xlsx
+++ b/hp1_clean.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>zinc_id</t>
   </si>
@@ -79,61 +79,64 @@
     <t>similarity</t>
   </si>
   <si>
-    <t>ZINC000257347364</t>
-  </si>
-  <si>
-    <t>NS(=O)(=O)c1ccc(NC2(O)OC(CO)C(O)C(O)C2O)cc1</t>
-  </si>
-  <si>
-    <t>ZINC000091746364</t>
-  </si>
-  <si>
-    <t>CC(O)C(N)C(=O)N1CCC2(CC1)c1nc[nH]c1CCN2S(C)(=O)=O</t>
+    <t>ZINC000001784491</t>
+  </si>
+  <si>
+    <t>COc1cc2ccc(=O)oc2c(OC2OC(CO)C(O)C(O)C2O)c1[O-]</t>
+  </si>
+  <si>
+    <t>ZINC000031156069</t>
+  </si>
+  <si>
+    <t>Cc1cc(=O)c2c(O)cc(OC3OC(CO)C(O)C(O)C3O)cc2o1</t>
+  </si>
+  <si>
+    <t>ZINC000008740325</t>
+  </si>
+  <si>
+    <t>CN1CCN(c2nc3c(N)ncnc3n2C2OC(CO)C(O)C2O)CC1</t>
   </si>
   <si>
     <t>ZINC000012652346</t>
   </si>
   <si>
-    <t>Cn1nc([O-])c(=O)nc1SCC1=C(C(=O)[O-])N2C(=O)C(N)C2SC1</t>
+    <t>Cn1nc([O-])c(=O)nc1SCC1=C(C(=O)[O-])N2C(=O)C([NH3+])C2SC1</t>
   </si>
   <si>
     <t>Cn1[n-]c(=O)c(=O)nc1SCC1=C(C(=O)[O-])N2C(=O)C(N)C2SC1</t>
   </si>
   <si>
-    <t>ZINC000091426318</t>
-  </si>
-  <si>
-    <t>CS(=O)(=O)N1CCc2nc[nH]c2C12CCN(C(=O)CNC(N)=O)CC2</t>
-  </si>
-  <si>
-    <t>ZINC000082096551</t>
-  </si>
-  <si>
-    <t>COCC(=O)N1CCN(C(=O)c2ncccc2[O-])C2CS(=O)(=O)CC21</t>
-  </si>
-  <si>
-    <t>ZINC000091894352</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)N2CC(C(=O)[O-])C(C3CC3)C2)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000091320034</t>
-  </si>
-  <si>
-    <t>O=C([O-])CCN1CCN(C(=O)c2c[nH]c(=O)cn2)C2CS(=O)(=O)CC21</t>
-  </si>
-  <si>
-    <t>ZINC000096163552</t>
-  </si>
-  <si>
-    <t>CS(=O)(=O)N1CC2CN(Cc3nc4ncccn4n3)CC2(C(=O)[O-])C1</t>
-  </si>
-  <si>
-    <t>ZINC000091563350</t>
-  </si>
-  <si>
-    <t>COCc1noc(CN2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)n1</t>
+    <t>Cn1[n-]c(=O)c(=O)nc1SCC1=C(C(=O)[O-])N2C(=O)C([NH3+])C2SC1</t>
+  </si>
+  <si>
+    <t>ZINC000020533355</t>
+  </si>
+  <si>
+    <t>CCN1CCN(Cc2nc3c(c(=O)n(C)c(=O)n3C)n2CC(N)=O)CC1</t>
+  </si>
+  <si>
+    <t>ZINC000020026470</t>
+  </si>
+  <si>
+    <t>COCCn1c(CN2CCN(C)CC2)nc2c1c(=O)n(C)c(=O)n2C</t>
+  </si>
+  <si>
+    <t>ZINC000022923851</t>
+  </si>
+  <si>
+    <t>CCN1CCN(Cc2nc3c(c(=O)n(C)c(=O)n3C)n2CCCO)CC1</t>
+  </si>
+  <si>
+    <t>ZINC000020026493</t>
+  </si>
+  <si>
+    <t>CN1CCN(Cc2nc3c(c(=O)n(C)c(=O)n3C)n2CCCO)CC1</t>
+  </si>
+  <si>
+    <t>ZINC000021700002</t>
+  </si>
+  <si>
+    <t>Cn1cc(S(=O)(=O)[N-]CCCOCC2CCCO2)c(=O)n(C)c1=O</t>
   </si>
   <si>
     <t>ZINC000077407345</t>
@@ -151,7 +154,7 @@
     <t>ZINC000071760227</t>
   </si>
   <si>
-    <t>O=C([O-])C1CN(S(=O)(=O)c2ccc(N3CCOCC3)nc2)CCN1</t>
+    <t>O=C([O-])C1CN(S(=O)(=O)c2ccc(N3CCOCC3)nc2)CC[NH2+]1</t>
   </si>
   <si>
     <t>ZINC000077389714</t>
@@ -160,10 +163,16 @@
     <t>COCC(=O)N1CCN(C(=O)c2cc(C)[nH]n2)C2CS(=O)(=O)CC21</t>
   </si>
   <si>
-    <t>ZINC000091745422</t>
-  </si>
-  <si>
-    <t>CCCS(=O)(=O)N1CCN(CCC(=O)[O-])C2CS(=O)(=O)CC21</t>
+    <t>ZINC000019358827</t>
+  </si>
+  <si>
+    <t>Cn1c(=O)c2c(ncn2CC(O)CN2CCN(CCO)CC2)n(C)c1=O</t>
+  </si>
+  <si>
+    <t>ZINC000017144342</t>
+  </si>
+  <si>
+    <t>Cn1c(N)c(S(=O)(=O)[N-]Cc2ccc3c(c2)OCO3)c(=O)n(C)c1=O</t>
   </si>
   <si>
     <t>ZINC000072411496</t>
@@ -172,28 +181,10 @@
     <t>CS(=O)(=O)N1CCOC(CNC(=O)CCc2cc3n(n2)CCNC3)C1</t>
   </si>
   <si>
-    <t>ZINC000096151859</t>
-  </si>
-  <si>
-    <t>CCS(=O)(=O)N1CC2CN(Cc3cc(=O)[nH]c(=O)[nH]3)CC2(C(=O)[O-])C1</t>
-  </si>
-  <si>
-    <t>ZINC000091690565</t>
-  </si>
-  <si>
-    <t>Cc1cnn(CC(=O)N2CC3CN(S(C)(=O)=O)CC3(C(=O)[O-])C2)c1</t>
-  </si>
-  <si>
-    <t>ZINC000077354184</t>
-  </si>
-  <si>
-    <t>O=C([O-])CN1CCN(Cc2nc(C(=O)[O-])co2)C2CS(=O)(=O)CC21</t>
-  </si>
-  <si>
-    <t>ZINC000091603058</t>
-  </si>
-  <si>
-    <t>COCc1nc(CN2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)no1</t>
+    <t>ZINC000015330957</t>
+  </si>
+  <si>
+    <t>CCOC(=O)N1CCC([N-]S(=O)(=O)c2cn(C)c(=O)n(C)c2=O)CC1</t>
   </si>
   <si>
     <t>ZINC000009307887</t>
@@ -202,46 +193,31 @@
     <t>CN(CCO)CCC(=O)NC1(C)CS(=O)(=O)CC1S(=O)(=O)[O-]</t>
   </si>
   <si>
-    <t>ZINC000001872264</t>
-  </si>
-  <si>
-    <t>Cn1c([O-])c(S(=O)c2c([O-])n(C)c(=O)n(C)c2=O)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000670472389</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)NCCN2CCCCC2CO)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000091988472</t>
-  </si>
-  <si>
-    <t>CN1CC(NC(=O)c2ccc(S(=O)(=O)NCCO)cc2)CC1CO</t>
-  </si>
-  <si>
-    <t>ZINC000077353848</t>
-  </si>
-  <si>
-    <t>O=C([O-])CN1CCN(C(=O)CCCn2cncn2)C2CS(=O)(=O)CC21</t>
-  </si>
-  <si>
-    <t>ZINC000670448199</t>
-  </si>
-  <si>
-    <t>Cn1cc(S(=O)(=O)NCCN2CCCC(CO)C2)c(=O)n(C)c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000091574424</t>
-  </si>
-  <si>
-    <t>O=C([O-])CCN1CCN(C(=O)N2CCOCC2)C2CS(=O)(=O)CC21</t>
-  </si>
-  <si>
-    <t>ZINC000092022362</t>
-  </si>
-  <si>
-    <t>CN1CCN(C(=O)N2CCN(CCC(=O)[O-])C3CS(=O)(=O)CC32)CC1</t>
+    <t>C[NH+](CCO)CCC(=O)NC1(C)CS(=O)(=O)CC1S(=O)(=O)[O-]</t>
+  </si>
+  <si>
+    <t>ZINC000077489412</t>
+  </si>
+  <si>
+    <t>O=C(c1cn(CCN2CC[NH2+]CC2)nn1)N1CCc2[n-][nH]c(=O)c2CC1</t>
+  </si>
+  <si>
+    <t>ZINC000077358035</t>
+  </si>
+  <si>
+    <t>O=C(Cc1cc(=O)[n-][nH]c1=O)N1CCOCC(O)(C[NH+]2CCCC2)C1</t>
+  </si>
+  <si>
+    <t>ZINC000004096261</t>
+  </si>
+  <si>
+    <t>NC(=O)C1CCCN1C(=O)C(Cc1cnc[nH]1)NC(=O)C1CCC(=O)N1</t>
+  </si>
+  <si>
+    <t>ZINC000005349782</t>
+  </si>
+  <si>
+    <t>CCOC(=O)CNC(=O)CNC(=O)CCCCc1c([O-])nc(N)[nH]c1=O</t>
   </si>
   <si>
     <t>ZINC000012687369</t>
@@ -250,22 +226,16 @@
     <t>Nc1cc(=O)[n-]c(SCC(=O)NC(=O)NC2CCS(=O)(=O)C2)n1</t>
   </si>
   <si>
-    <t>ZINC000011905809</t>
-  </si>
-  <si>
-    <t>NS(=O)(=O)c1ccc(NC(=O)CSc2n[nH]c(=O)[n-]c2=O)cc1</t>
-  </si>
-  <si>
-    <t>ZINC000091288550</t>
-  </si>
-  <si>
-    <t>Cn1nnnc1SCCNC(=O)c1cnc(Cn2cncn2)[n-]c1=O</t>
-  </si>
-  <si>
-    <t>ZINC000330730473</t>
-  </si>
-  <si>
-    <t>CN(C)CC(=O)N1CCN(S(=O)(=O)CCCN2CCOCC2)CC1</t>
+    <t>ZINC000091391068</t>
+  </si>
+  <si>
+    <t>O=C(NCc1n[nH]c(=O)[n-]1)C1CCC(=O)N(CCC[NH+]2CCOCC2)C1</t>
+  </si>
+  <si>
+    <t>ZINC000013562447</t>
+  </si>
+  <si>
+    <t>CCN(CC(O)C[NH+](C)CC(O)CN1CCOCC1)S(=O)(=O)[O-]</t>
   </si>
   <si>
     <t>ZINC000035552524</t>
@@ -274,10 +244,22 @@
     <t>CS(=O)(=O)N(CCCN1CCOCC1)CCC(=O)N1CCNCC1</t>
   </si>
   <si>
-    <t>ZINC000006095847</t>
-  </si>
-  <si>
-    <t>O=C([O-])CNC(=O)CNC(=O)CNC(=O)CSC(=O)c1ccccc1</t>
+    <t>ZINC000002973678</t>
+  </si>
+  <si>
+    <t>CC(NC(=O)C(N)Cc1ccc(O)cc1)C(=O)NCC(=O)NCC(N)=O</t>
+  </si>
+  <si>
+    <t>ZINC000019370490</t>
+  </si>
+  <si>
+    <t>O=S(=O)([O-])CC(O)CN1CC[NH+](CC(O)CS(=O)(=O)[O-])CC1</t>
+  </si>
+  <si>
+    <t>ZINC000003896107</t>
+  </si>
+  <si>
+    <t>OCCN1CCOCCOCCOCCN(CCO)CCOCC1</t>
   </si>
 </sst>
 </file>
@@ -1533,82 +1515,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1219200" y="118300500"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33" descr="f"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1219200" y="122110500"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34" descr="f"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1219200" y="125920500"/>
           <a:ext cx="2857500" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1906,7 +1812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1988,58 +1894,58 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>0.5846432169582619</v>
+        <v>0.2820677847427193</v>
       </c>
       <c r="E2">
-        <v>0.985893414103122</v>
+        <v>0.9345340044318243</v>
       </c>
       <c r="F2">
-        <v>0.001121872241738584</v>
+        <v>0.0005133629861150913</v>
       </c>
       <c r="G2">
-        <v>0.1673743589325732</v>
+        <v>0.3558738464127689</v>
       </c>
       <c r="H2">
-        <v>0.9594063749865595</v>
+        <v>0.7789343537405304</v>
       </c>
       <c r="I2">
-        <v>855.1832724729431</v>
+        <v>1517.316937154289</v>
       </c>
       <c r="J2">
-        <v>4901.995076336246</v>
+        <v>3321.093414914771</v>
       </c>
       <c r="K2">
-        <v>5109.404319316639</v>
+        <v>4263.637107500146</v>
       </c>
       <c r="L2">
-        <v>4.043850394446073</v>
+        <v>3.594850531105379</v>
       </c>
       <c r="M2">
-        <v>0.192178247936826</v>
+        <v>0.1771102511488565</v>
       </c>
       <c r="N2">
-        <v>352.4160000000002</v>
+        <v>369.302</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R2">
-        <v>112.81</v>
+        <v>161.88</v>
       </c>
       <c r="S2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U2">
-        <v>0.3979148566463944</v>
+        <v>0.3746130030959752</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="300" customHeight="1">
@@ -2050,58 +1956,58 @@
         <v>24</v>
       </c>
       <c r="D3">
-        <v>0.4906594722358194</v>
+        <v>0.4966831097558905</v>
       </c>
       <c r="E3">
-        <v>0.9767682080392288</v>
+        <v>0.9775528060829043</v>
       </c>
       <c r="F3">
-        <v>0.0009177723299327842</v>
+        <v>0.0007700470216373529</v>
       </c>
       <c r="G3">
-        <v>0.2142985482074799</v>
+        <v>0.2106905582114201</v>
       </c>
       <c r="H3">
-        <v>0.8932374660082714</v>
+        <v>0.8817870144690986</v>
       </c>
       <c r="I3">
-        <v>973.2669387338036</v>
+        <v>1145.10801248754</v>
       </c>
       <c r="J3">
-        <v>4056.763339630809</v>
+        <v>4792.5326324438</v>
       </c>
       <c r="K3">
-        <v>4541.640374490566</v>
+        <v>5435.022918010719</v>
       </c>
       <c r="L3">
-        <v>3.728355380948158</v>
+        <v>4.112338221601836</v>
       </c>
       <c r="M3">
-        <v>0.154886579713828</v>
+        <v>0.1305717597064652</v>
       </c>
       <c r="N3">
-        <v>364.4490000000002</v>
+        <v>355.3960000000002</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>131.57</v>
+        <v>114.9</v>
       </c>
       <c r="S3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U3">
-        <v>0.314359637774903</v>
+        <v>0.3690851735015773</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="300" customHeight="1">
@@ -2112,722 +2018,722 @@
         <v>26</v>
       </c>
       <c r="D4">
-        <v>0.3449552659626504</v>
+        <v>0.4506626931303094</v>
       </c>
       <c r="E4">
-        <v>0.9510808943401239</v>
+        <v>0.9715589404912564</v>
       </c>
       <c r="F4">
-        <v>0.0005577448750631422</v>
+        <v>0.0007393290426064017</v>
       </c>
       <c r="G4">
-        <v>0.3089419563950321</v>
+        <v>0.2367978571514265</v>
       </c>
       <c r="H4">
-        <v>0.7611068055412593</v>
+        <v>0.8411829048932238</v>
       </c>
       <c r="I4">
-        <v>1364.614610676781</v>
+        <v>1137.765266095527</v>
       </c>
       <c r="J4">
-        <v>3361.853078314471</v>
+        <v>4041.711792217886</v>
       </c>
       <c r="K4">
-        <v>4417.058228672252</v>
+        <v>4804.795447823472</v>
       </c>
       <c r="L4">
-        <v>3.633519713547636</v>
+        <v>3.819337030262012</v>
       </c>
       <c r="M4">
-        <v>0.1086263544986856</v>
+        <v>0.1151699784515435</v>
       </c>
       <c r="N4">
-        <v>363.4170000000001</v>
+        <v>357.3440000000001</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>117.86</v>
+        <v>146.91</v>
       </c>
       <c r="S4">
         <v>11</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U4">
-        <v>0.308381317978247</v>
+        <v>0.3285266457680251</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="300" customHeight="1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>0.4309271650985923</v>
+        <v>0.2530590570887533</v>
       </c>
       <c r="E5">
-        <v>0.9685243186049406</v>
+        <v>0.9249919988661561</v>
       </c>
       <c r="F5">
-        <v>0.0006926963921350542</v>
+        <v>0.0007164821040708812</v>
       </c>
       <c r="G5">
-        <v>0.2489189512086924</v>
+        <v>0.3799865813862289</v>
       </c>
       <c r="H5">
-        <v>0.8237015423531667</v>
+        <v>0.8636450802572696</v>
       </c>
       <c r="I5">
-        <v>1189.12347704645</v>
+        <v>1205.396583320425</v>
       </c>
       <c r="J5">
-        <v>3934.946846495138</v>
+        <v>2739.662082660415</v>
       </c>
       <c r="K5">
-        <v>4777.151242492158</v>
+        <v>3172.208289363846</v>
       </c>
       <c r="L5">
-        <v>3.717135664444417</v>
+        <v>3.262818599702426</v>
       </c>
       <c r="M5">
-        <v>0.1090918048168907</v>
+        <v>0.3777910153940038</v>
       </c>
       <c r="N5">
-        <v>369.3840000000001</v>
+        <v>350.3980000000001</v>
       </c>
       <c r="O5">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="P5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>152.52</v>
+        <v>126.38</v>
       </c>
       <c r="S5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5">
-        <v>0.3069498069498069</v>
+        <v>0.308381317978247</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="300" customHeight="1">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="D6">
-        <v>0.7722535688004022</v>
+        <v>0.4309271650985923</v>
       </c>
       <c r="E6">
-        <v>0.9965611605726561</v>
+        <v>0.9685243186049406</v>
       </c>
       <c r="F6">
-        <v>0.001372657827770624</v>
+        <v>0.0006926963921350542</v>
       </c>
       <c r="G6">
-        <v>0.08286044435121516</v>
+        <v>0.2489189512086924</v>
       </c>
       <c r="H6">
-        <v>0.9515155028443129</v>
+        <v>0.8237015423531667</v>
       </c>
       <c r="I6">
-        <v>693.192056748548</v>
+        <v>1189.12347704645</v>
       </c>
       <c r="J6">
-        <v>7960.167165518045</v>
+        <v>3934.946846495138</v>
       </c>
       <c r="K6">
-        <v>8365.777690140787</v>
+        <v>4777.151242492158</v>
       </c>
       <c r="L6">
-        <v>4.971554384167305</v>
+        <v>3.717135664444417</v>
       </c>
       <c r="M6">
-        <v>0.05094549195576247</v>
+        <v>0.1090918048168907</v>
       </c>
       <c r="N6">
-        <v>360.4170000000001</v>
+        <v>369.3840000000001</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Q6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>133.8</v>
+        <v>152.52</v>
       </c>
       <c r="S6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U6">
-        <v>0.3051398828887443</v>
+        <v>0.3069498069498069</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="300" customHeight="1">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
       <c r="D7">
-        <v>0.5708675857338262</v>
+        <v>0.5756321208056376</v>
       </c>
       <c r="E7">
-        <v>0.9850930317828652</v>
+        <v>0.9855280088791096</v>
       </c>
       <c r="F7">
-        <v>0.001063572838338249</v>
+        <v>0.0008698721792981615</v>
       </c>
       <c r="G7">
-        <v>0.1720224367134792</v>
+        <v>0.1695126653521137</v>
       </c>
       <c r="H7">
-        <v>0.8992785886654669</v>
+        <v>0.8732194419625041</v>
       </c>
       <c r="I7">
-        <v>845.5260949222062</v>
+        <v>1003.847993698388</v>
       </c>
       <c r="J7">
-        <v>4420.141510888651</v>
+        <v>5171.174573012844</v>
       </c>
       <c r="K7">
-        <v>4915.208219788886</v>
+        <v>5921.96454237318</v>
       </c>
       <c r="L7">
-        <v>3.914077247657001</v>
+        <v>4.22876641150426</v>
       </c>
       <c r="M7">
-        <v>0.1225464180700887</v>
+        <v>0.06062294014354769</v>
       </c>
       <c r="N7">
-        <v>352.4340000000001</v>
+        <v>360.4120000000001</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>108.9</v>
+        <v>110.7</v>
       </c>
       <c r="S7">
         <v>10</v>
       </c>
       <c r="T7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="U7">
-        <v>0.2851959361393324</v>
+        <v>0.3069498069498069</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="300" customHeight="1">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8">
-        <v>0.5370800285465821</v>
+        <v>0.5057764024197648</v>
       </c>
       <c r="E8">
-        <v>0.9819813035158284</v>
+        <v>0.9786358209323618</v>
       </c>
       <c r="F8">
-        <v>0.0008907438088225321</v>
+        <v>0.0006841619366974537</v>
       </c>
       <c r="G8">
-        <v>0.1889780927656821</v>
+        <v>0.2056013861530175</v>
       </c>
       <c r="H8">
-        <v>0.8704297112809343</v>
+        <v>0.8731870878868605</v>
       </c>
       <c r="I8">
-        <v>977.1942310006613</v>
+        <v>1276.287149358028</v>
       </c>
       <c r="J8">
-        <v>4500.939129542125</v>
+        <v>5420.379113718359</v>
       </c>
       <c r="K8">
-        <v>5170.939216813373</v>
+        <v>6207.580470338656</v>
       </c>
       <c r="L8">
-        <v>3.955972979567874</v>
+        <v>4.380953308385985</v>
       </c>
       <c r="M8">
-        <v>0.08898898629685369</v>
+        <v>0.1147721345617283</v>
       </c>
       <c r="N8">
-        <v>360.3920000000001</v>
+        <v>359.3590000000001</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R8">
-        <v>119.71</v>
+        <v>195.2</v>
       </c>
       <c r="S8">
         <v>11</v>
       </c>
       <c r="T8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U8">
-        <v>0.2759365994236311</v>
+        <v>0.29155672823219</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="300" customHeight="1">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
       <c r="D9">
-        <v>0.498885079185205</v>
+        <v>0.2825777336052872</v>
       </c>
       <c r="E9">
-        <v>0.9777534653167165</v>
+        <v>0.9305832272519482</v>
       </c>
       <c r="F9">
-        <v>0.0007580775527358738</v>
+        <v>0.0004446789774957031</v>
       </c>
       <c r="G9">
-        <v>0.2097573861897419</v>
+        <v>0.3660803971224748</v>
       </c>
       <c r="H9">
-        <v>0.8946863957121091</v>
+        <v>0.7004624944990858</v>
       </c>
       <c r="I9">
-        <v>1180.204310869276</v>
+        <v>1575.209375635155</v>
       </c>
       <c r="J9">
-        <v>5033.971676879928</v>
+        <v>3014.023961098923</v>
       </c>
       <c r="K9">
-        <v>5626.52086921835</v>
+        <v>4302.905558497189</v>
       </c>
       <c r="L9">
-        <v>4.099302010316602</v>
+        <v>3.636726002999578</v>
       </c>
       <c r="M9">
-        <v>0.1718575465412039</v>
+        <v>0.09480409107237293</v>
       </c>
       <c r="N9">
-        <v>374.4880000000001</v>
+        <v>357.335</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R9">
-        <v>116.83</v>
+        <v>148.74</v>
       </c>
       <c r="S9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U9">
-        <v>0.2732778198334595</v>
+        <v>0.2914438502673797</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="300" customHeight="1">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
       <c r="D10">
-        <v>0.4701098577918231</v>
+        <v>0.7891522600010961</v>
       </c>
       <c r="E10">
-        <v>0.9741853374449321</v>
+        <v>0.9970706897467758</v>
       </c>
       <c r="F10">
-        <v>0.0006738366626951883</v>
+        <v>0.001581783609356686</v>
       </c>
       <c r="G10">
-        <v>0.2257497027845301</v>
+        <v>0.07648555188981104</v>
       </c>
       <c r="H10">
-        <v>0.8311971174795549</v>
+        <v>0.9732289779115229</v>
       </c>
       <c r="I10">
-        <v>1233.529078330291</v>
+        <v>615.273146184222</v>
       </c>
       <c r="J10">
-        <v>4541.781457909459</v>
+        <v>7828.951225454206</v>
       </c>
       <c r="K10">
-        <v>5464.144860946506</v>
+        <v>8044.305505837438</v>
       </c>
       <c r="L10">
-        <v>4.017065896801048</v>
+        <v>4.981751255632142</v>
       </c>
       <c r="M10">
-        <v>0.08913781512818016</v>
+        <v>0.07043294960988521</v>
       </c>
       <c r="N10">
-        <v>370.4310000000002</v>
+        <v>349.3270000000001</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>119.39</v>
+        <v>140.56</v>
       </c>
       <c r="S10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T10">
         <v>5</v>
       </c>
       <c r="U10">
-        <v>0.2693156732891832</v>
+        <v>0.2907754010695187</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="300" customHeight="1">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
       <c r="D11">
-        <v>0.5924543544911338</v>
+        <v>0.394495921955718</v>
       </c>
       <c r="E11">
-        <v>0.9866363473260849</v>
+        <v>0.9621060110927967</v>
       </c>
       <c r="F11">
-        <v>0.001087280961573521</v>
+        <v>0.000789438086803199</v>
       </c>
       <c r="G11">
-        <v>0.1629377738127083</v>
+        <v>0.2726756744176263</v>
       </c>
       <c r="H11">
-        <v>0.9494030519616842</v>
+        <v>0.8922441781772852</v>
       </c>
       <c r="I11">
-        <v>873.1901739433578</v>
+        <v>1130.226921012129</v>
       </c>
       <c r="J11">
-        <v>5087.88966908126</v>
+        <v>3698.307127858424</v>
       </c>
       <c r="K11">
-        <v>5359.040776800237</v>
+        <v>4144.949575813972</v>
       </c>
       <c r="L11">
-        <v>4.031455303526324</v>
+        <v>3.631843365199452</v>
       </c>
       <c r="M11">
-        <v>0.1759729182455492</v>
+        <v>0.2196240100478567</v>
       </c>
       <c r="N11">
-        <v>372.4470000000001</v>
+        <v>359.307</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R11">
-        <v>110.48</v>
+        <v>157.97</v>
       </c>
       <c r="S11">
         <v>10</v>
       </c>
       <c r="T11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U11">
-        <v>0.2663438256658596</v>
+        <v>0.2906898861352981</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="300" customHeight="1">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
       <c r="D12">
-        <v>0.6657056224767195</v>
+        <v>0.396330582396856</v>
       </c>
       <c r="E12">
-        <v>0.9918386362210143</v>
+        <v>0.9619556116721586</v>
       </c>
       <c r="F12">
-        <v>0.001174263379651534</v>
+        <v>0.0007476315331561809</v>
       </c>
       <c r="G12">
-        <v>0.127499489015598</v>
+        <v>0.2732057853934344</v>
       </c>
       <c r="H12">
-        <v>0.9140280285056589</v>
+        <v>0.9208743281605791</v>
       </c>
       <c r="I12">
-        <v>778.3841720218675</v>
+        <v>1231.722161681759</v>
       </c>
       <c r="J12">
-        <v>5580.139619901677</v>
+        <v>4151.673861831934</v>
       </c>
       <c r="K12">
-        <v>6104.998365339658</v>
+        <v>4508.404387952466</v>
       </c>
       <c r="L12">
-        <v>4.230134954038514</v>
+        <v>3.812699194564094</v>
       </c>
       <c r="M12">
-        <v>0.06960301393463061</v>
+        <v>0.2574193412402511</v>
       </c>
       <c r="N12">
-        <v>370.4350000000002</v>
+        <v>357.3720000000001</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>102.44</v>
+        <v>132.18</v>
       </c>
       <c r="S12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U12">
-        <v>0.2637277648878577</v>
+        <v>0.2690058479532164</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="300" customHeight="1">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
       <c r="D13">
-        <v>0.4663352874565803</v>
+        <v>0.6563133425955976</v>
       </c>
       <c r="E13">
-        <v>0.9730357331053255</v>
+        <v>0.9910258417277895</v>
       </c>
       <c r="F13">
-        <v>0.0009242504873416692</v>
+        <v>0.001144897433213243</v>
       </c>
       <c r="G13">
-        <v>0.2306544213757487</v>
+        <v>0.133670419419281</v>
       </c>
       <c r="H13">
-        <v>0.9398661374015223</v>
+        <v>0.9756336220010454</v>
       </c>
       <c r="I13">
-        <v>1016.895473979967</v>
+        <v>852.1581005408093</v>
       </c>
       <c r="J13">
-        <v>4143.625843242259</v>
+        <v>6219.731319465272</v>
       </c>
       <c r="K13">
-        <v>4408.740434779652</v>
+        <v>6375.06865200942</v>
       </c>
       <c r="L13">
-        <v>3.706598443578781</v>
+        <v>4.406362146347631</v>
       </c>
       <c r="M13">
-        <v>0.2293665451897019</v>
+        <v>0.1585093390426654</v>
       </c>
       <c r="N13">
-        <v>374.4630000000002</v>
+        <v>362.4130000000001</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P13">
         <v>8</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13">
-        <v>102.64</v>
+        <v>148.76</v>
       </c>
       <c r="S13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U13">
-        <v>0.2636080870917574</v>
+        <v>0.2637277648878577</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="300" customHeight="1">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
       <c r="D14">
-        <v>0.4984411504578892</v>
+        <v>0.6017755503611276</v>
       </c>
       <c r="E14">
-        <v>0.977623809770786</v>
+        <v>0.9874326396828513</v>
       </c>
       <c r="F14">
-        <v>0.0009057621926329796</v>
+        <v>0.001296579691458133</v>
       </c>
       <c r="G14">
-        <v>0.2103608484705597</v>
+        <v>0.1580404444721544</v>
       </c>
       <c r="H14">
-        <v>0.9058309327648238</v>
+        <v>0.9426011076270576</v>
       </c>
       <c r="I14">
-        <v>1000.075892030384</v>
+        <v>726.990491858629</v>
       </c>
       <c r="J14">
-        <v>4306.408177661814</v>
+        <v>4335.991620050279</v>
       </c>
       <c r="K14">
-        <v>4754.09706369551</v>
+        <v>4600.028140181037</v>
       </c>
       <c r="L14">
-        <v>3.879331833145499</v>
+        <v>3.801828496836952</v>
       </c>
       <c r="M14">
-        <v>0.1696517532485974</v>
+        <v>0.1502536602683621</v>
       </c>
       <c r="N14">
-        <v>357.4400000000001</v>
+        <v>352.4140000000002</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>104.53</v>
+        <v>127.25</v>
       </c>
       <c r="S14">
         <v>11</v>
       </c>
       <c r="T14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U14">
-        <v>0.2626339969372128</v>
+        <v>0.2636080870917574</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="300" customHeight="1">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
       <c r="D15">
-        <v>0.7762901422904512</v>
+        <v>0.2260349709716991</v>
       </c>
       <c r="E15">
-        <v>0.9966588676495182</v>
+        <v>0.8966663144470005</v>
       </c>
       <c r="F15">
-        <v>0.001866376355933924</v>
+        <v>0.0003164735386262744</v>
       </c>
       <c r="G15">
-        <v>0.08167681149249317</v>
+        <v>0.4427070369172291</v>
       </c>
       <c r="H15">
-        <v>0.9739419885855243</v>
+        <v>0.6264526410946241</v>
       </c>
       <c r="I15">
-        <v>521.8357945271812</v>
+        <v>1979.478738771919</v>
       </c>
       <c r="J15">
-        <v>6222.546915701055</v>
+        <v>2801.061606179463</v>
       </c>
       <c r="K15">
-        <v>6389.032394771465</v>
+        <v>4471.306244770655</v>
       </c>
       <c r="L15">
-        <v>4.432378406814022</v>
+        <v>3.698190671437479</v>
       </c>
       <c r="M15">
-        <v>0.08605198427876341</v>
+        <v>0.09925878151944256</v>
       </c>
       <c r="N15">
-        <v>351.3880000000001</v>
+        <v>360.4120000000001</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P15">
         <v>7</v>
@@ -2836,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>105.47</v>
+        <v>110.29</v>
       </c>
       <c r="S15">
         <v>10</v>
@@ -2845,438 +2751,438 @@
         <v>3</v>
       </c>
       <c r="U15">
-        <v>0.2620997766195086</v>
+        <v>0.2626339969372128</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="300" customHeight="1">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
       <c r="D16">
-        <v>0.4521946896802228</v>
+        <v>0.5855159790802941</v>
       </c>
       <c r="E16">
-        <v>0.9717963302796065</v>
+        <v>0.9863262826529224</v>
       </c>
       <c r="F16">
-        <v>0.0006609068887957628</v>
+        <v>0.0009981455058712776</v>
       </c>
       <c r="G16">
-        <v>0.2358217387245924</v>
+        <v>0.1648043207809412</v>
       </c>
       <c r="H16">
-        <v>0.8509425515174648</v>
+        <v>0.9013321751687305</v>
       </c>
       <c r="I16">
-        <v>1287.53772421402</v>
+        <v>903.0067959700535</v>
       </c>
       <c r="J16">
-        <v>4645.969630039931</v>
+        <v>4938.639204039358</v>
       </c>
       <c r="K16">
-        <v>5459.792346445583</v>
+        <v>5479.266512498391</v>
       </c>
       <c r="L16">
-        <v>4.01015885182064</v>
+        <v>4.03157315722799</v>
       </c>
       <c r="M16">
-        <v>0.1218556277968444</v>
+        <v>0.09799814198626905</v>
       </c>
       <c r="N16">
-        <v>373.3910000000001</v>
+        <v>365.3950000000002</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P16">
         <v>9</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>148.93</v>
+        <v>123.83</v>
       </c>
       <c r="S16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U16">
-        <v>0.2596078431372549</v>
+        <v>0.2620997766195086</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="300" customHeight="1">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
       <c r="D17">
-        <v>0.6195773890165506</v>
+        <v>0.1965139361680568</v>
       </c>
       <c r="E17">
-        <v>0.9889088623450888</v>
+        <v>0.9001258023046834</v>
       </c>
       <c r="F17">
-        <v>0.001050461832639103</v>
+        <v>0.0005410256737995875</v>
       </c>
       <c r="G17">
-        <v>0.1485236074681138</v>
+        <v>0.4356300494976787</v>
       </c>
       <c r="H17">
-        <v>0.906372970627521</v>
+        <v>0.8017381047225275</v>
       </c>
       <c r="I17">
-        <v>862.8328440552818</v>
+        <v>1481.885506637742</v>
       </c>
       <c r="J17">
-        <v>5265.481907913356</v>
+        <v>2727.277603731643</v>
       </c>
       <c r="K17">
-        <v>5809.398645535332</v>
+        <v>3401.706352320029</v>
       </c>
       <c r="L17">
-        <v>4.139967158683688</v>
+        <v>3.325048370825103</v>
       </c>
       <c r="M17">
-        <v>0.08812684507888002</v>
+        <v>0.2959196482958288</v>
       </c>
       <c r="N17">
-        <v>366.3990000000001</v>
+        <v>357.3020000000001</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P17">
         <v>8</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R17">
-        <v>120.13</v>
+        <v>152.69</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U17">
-        <v>0.2589147286821705</v>
+        <v>0.2598540145985401</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="300" customHeight="1">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
       <c r="D18">
-        <v>0.4379754417308929</v>
+        <v>0.2759317873362557</v>
       </c>
       <c r="E18">
-        <v>0.9696875734366118</v>
+        <v>0.929057316621295</v>
       </c>
       <c r="F18">
-        <v>0.0006084950156751938</v>
+        <v>0.0003712081545691443</v>
       </c>
       <c r="G18">
-        <v>0.2443481326358271</v>
+        <v>0.3699358085295862</v>
       </c>
       <c r="H18">
-        <v>0.8404205452837877</v>
+        <v>0.709716938847242</v>
       </c>
       <c r="I18">
-        <v>1381.146145217388</v>
+        <v>1911.910959151745</v>
       </c>
       <c r="J18">
-        <v>4750.368189676956</v>
+        <v>3667.97580010195</v>
       </c>
       <c r="K18">
-        <v>5652.37037139886</v>
+        <v>5168.223554111109</v>
       </c>
       <c r="L18">
-        <v>4.101493545933755</v>
+        <v>3.951362632895221</v>
       </c>
       <c r="M18">
-        <v>0.1205180511638987</v>
+        <v>0.1178839750850315</v>
       </c>
       <c r="N18">
-        <v>371.4150000000001</v>
+        <v>373.4300000000002</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R18">
-        <v>114.04</v>
+        <v>144.54</v>
       </c>
       <c r="S18">
         <v>10</v>
       </c>
       <c r="T18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U18">
-        <v>0.2556221889055472</v>
+        <v>0.2597669636737491</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="300" customHeight="1">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
       <c r="D19">
-        <v>0.6670259344653984</v>
+        <v>0.7201415452874401</v>
       </c>
       <c r="E19">
-        <v>0.9918150557458995</v>
+        <v>0.9945222021967041</v>
       </c>
       <c r="F19">
-        <v>0.001170080156105049</v>
+        <v>0.001553362374556717</v>
       </c>
       <c r="G19">
-        <v>0.1276827913062611</v>
+        <v>0.1045255439489216</v>
       </c>
       <c r="H19">
-        <v>0.9503417957563013</v>
+        <v>0.9556692073169601</v>
       </c>
       <c r="I19">
-        <v>812.2023015241872</v>
+        <v>615.2261848042247</v>
       </c>
       <c r="J19">
-        <v>6045.213970115071</v>
+        <v>5624.966856329447</v>
       </c>
       <c r="K19">
-        <v>6361.094500010038</v>
+        <v>5885.893166027116</v>
       </c>
       <c r="L19">
-        <v>4.356373348898332</v>
+        <v>4.246372182194109</v>
       </c>
       <c r="M19">
-        <v>0.1148041413675377</v>
+        <v>0.09167617937287313</v>
       </c>
       <c r="N19">
-        <v>366.4030000000001</v>
+        <v>355.3960000000002</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19">
-        <v>120.05</v>
+        <v>115.64</v>
       </c>
       <c r="S19">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T19">
         <v>4</v>
       </c>
       <c r="U19">
-        <v>0.2548262548262548</v>
+        <v>0.2589147286821705</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="300" customHeight="1">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
       <c r="D20">
-        <v>0.2267249140963487</v>
+        <v>0.5863692812514322</v>
       </c>
       <c r="E20">
-        <v>0.9113676632772407</v>
+        <v>0.9864026090519522</v>
       </c>
       <c r="F20">
-        <v>0.0004094361628664221</v>
+        <v>0.001057630020002306</v>
       </c>
       <c r="G20">
-        <v>0.4115932243521288</v>
+        <v>0.1643468674952505</v>
       </c>
       <c r="H20">
-        <v>0.7314961632279725</v>
+        <v>0.8985049802092273</v>
       </c>
       <c r="I20">
-        <v>1786.593929824958</v>
+        <v>849.5456475481556</v>
       </c>
       <c r="J20">
-        <v>3175.18979320045</v>
+        <v>4644.572828619018</v>
       </c>
       <c r="K20">
-        <v>4340.678670396382</v>
+        <v>5169.223244079822</v>
       </c>
       <c r="L20">
-        <v>3.730349773446264</v>
+        <v>3.982484795506519</v>
       </c>
       <c r="M20">
-        <v>0.2102725624910737</v>
+        <v>0.08689975441537842</v>
       </c>
       <c r="N20">
-        <v>361.4640000000001</v>
+        <v>353.3030000000001</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P20">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R20">
-        <v>87.22999999999999</v>
+        <v>152.65</v>
       </c>
       <c r="S20">
         <v>9</v>
       </c>
       <c r="T20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U20">
-        <v>0.2534142640364188</v>
+        <v>0.2540792540792541</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="300" customHeight="1">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
       <c r="D21">
-        <v>0.7198834740868743</v>
+        <v>0.6252209871577864</v>
       </c>
       <c r="E21">
-        <v>0.9944361521023837</v>
+        <v>0.9893006668386348</v>
       </c>
       <c r="F21">
-        <v>0.001346891739418987</v>
+        <v>0.0008152271922343066</v>
       </c>
       <c r="G21">
-        <v>0.1053410622302858</v>
+        <v>0.1458910230022134</v>
       </c>
       <c r="H21">
-        <v>0.9771329643189174</v>
+        <v>0.9072936966316004</v>
       </c>
       <c r="I21">
-        <v>725.472534815921</v>
+        <v>1112.933554319951</v>
       </c>
       <c r="J21">
-        <v>6729.409343974076</v>
+        <v>6921.314127662086</v>
       </c>
       <c r="K21">
-        <v>6886.892152558397</v>
+        <v>7628.526631848113</v>
       </c>
       <c r="L21">
-        <v>4.537642506676654</v>
+        <v>4.755569219745914</v>
       </c>
       <c r="M21">
-        <v>0.09357795293439249</v>
+        <v>0.08024936629383699</v>
       </c>
       <c r="N21">
-        <v>362.379</v>
+        <v>360.3970000000001</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P21">
+        <v>8</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>162.42</v>
+      </c>
+      <c r="S21">
         <v>12</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>138.3</v>
-      </c>
-      <c r="S21">
-        <v>13</v>
-      </c>
       <c r="T21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U21">
-        <v>0.2479806138933764</v>
+        <v>0.246422893481717</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="300" customHeight="1">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22">
-        <v>0.611904032504493</v>
+        <v>0.7103829879530523</v>
       </c>
       <c r="E22">
-        <v>0.9883260469454799</v>
+        <v>0.9939330105800347</v>
       </c>
       <c r="F22">
-        <v>0.0009119892525715434</v>
+        <v>0.001232367292209485</v>
       </c>
       <c r="G22">
-        <v>0.1523536180375151</v>
+        <v>0.1099871377903282</v>
       </c>
       <c r="H22">
-        <v>0.9177898546827249</v>
+        <v>0.9889033990602704</v>
       </c>
       <c r="I22">
-        <v>1006.360384286137</v>
+        <v>802.4421009156177</v>
       </c>
       <c r="J22">
-        <v>6062.391971715388</v>
+        <v>7214.82290644988</v>
       </c>
       <c r="K22">
-        <v>6605.424913757763</v>
+        <v>7295.781279855992</v>
       </c>
       <c r="L22">
-        <v>4.443575476855749</v>
+        <v>4.716760292182724</v>
       </c>
       <c r="M22">
-        <v>0.1139950280633552</v>
+        <v>0.1358021007103939</v>
       </c>
       <c r="N22">
-        <v>371.4630000000002</v>
+        <v>358.2590000000001</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="P22">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q22">
         <v>2</v>
       </c>
       <c r="R22">
-        <v>105.56</v>
+        <v>218.72</v>
       </c>
       <c r="S22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T22">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U22">
         <v>0.246422893481717</v>
@@ -3284,117 +3190,117 @@
     </row>
     <row r="23" spans="1:21" ht="300" customHeight="1">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23">
-        <v>0.2655372629737516</v>
+        <v>0.5245539249639466</v>
       </c>
       <c r="E23">
-        <v>0.9213422831385801</v>
+        <v>0.9803358589625273</v>
       </c>
       <c r="F23">
-        <v>0.0003645423499363801</v>
+        <v>0.001090759493690544</v>
       </c>
       <c r="G23">
-        <v>0.3887523598654915</v>
+        <v>0.1973362704426222</v>
       </c>
       <c r="H23">
-        <v>0.6682841852922914</v>
+        <v>0.9345320861581436</v>
       </c>
       <c r="I23">
-        <v>1833.214125626063</v>
+        <v>856.7719021139935</v>
       </c>
       <c r="J23">
-        <v>3151.384106926635</v>
+        <v>4057.443830515072</v>
       </c>
       <c r="K23">
-        <v>4715.634719903323</v>
+        <v>4341.684882319239</v>
       </c>
       <c r="L23">
-        <v>3.731877710580078</v>
+        <v>3.732426473811897</v>
       </c>
       <c r="M23">
-        <v>0.08365118004526625</v>
+        <v>0.204777536120134</v>
       </c>
       <c r="N23">
-        <v>368.4150000000001</v>
+        <v>349.341</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R23">
-        <v>109.77</v>
+        <v>184.64</v>
       </c>
       <c r="S23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U23">
-        <v>0.2431192660550459</v>
+        <v>0.2352059925093633</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="300" customHeight="1">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24">
-        <v>0.4133532567733383</v>
+        <v>0.3516779882697849</v>
       </c>
       <c r="E24">
-        <v>0.9655618938301685</v>
+        <v>0.9536788214993958</v>
       </c>
       <c r="F24">
-        <v>0.0006018782602284369</v>
+        <v>0.0007716035115857234</v>
       </c>
       <c r="G24">
-        <v>0.2601734597976865</v>
+        <v>0.3008267033086053</v>
       </c>
       <c r="H24">
-        <v>0.8101135269594429</v>
+        <v>0.8587449869516375</v>
       </c>
       <c r="I24">
-        <v>1345.975723814933</v>
+        <v>1112.935560890372</v>
       </c>
       <c r="J24">
-        <v>4191.023718058734</v>
+        <v>3177.004644878135</v>
       </c>
       <c r="K24">
-        <v>5173.37827179443</v>
+        <v>3699.590324428941</v>
       </c>
       <c r="L24">
-        <v>3.932641446347698</v>
+        <v>3.436653270379291</v>
       </c>
       <c r="M24">
-        <v>0.1026332091942189</v>
+        <v>0.1985319025944983</v>
       </c>
       <c r="N24">
-        <v>367.4310000000002</v>
+        <v>356.3800000000002</v>
       </c>
       <c r="O24">
+        <v>-1</v>
+      </c>
+      <c r="P24">
+        <v>8</v>
+      </c>
+      <c r="Q24">
         <v>0</v>
       </c>
-      <c r="P24">
-        <v>6</v>
-      </c>
-      <c r="Q24">
-        <v>2</v>
-      </c>
       <c r="R24">
-        <v>125.7</v>
+        <v>121.51</v>
       </c>
       <c r="S24">
         <v>10</v>
@@ -3403,689 +3309,565 @@
         <v>4</v>
       </c>
       <c r="U24">
-        <v>0.239558707643814</v>
+        <v>0.2348993288590604</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="300" customHeight="1">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25">
-        <v>0.706257657528879</v>
+        <v>0.7705903412312599</v>
       </c>
       <c r="E25">
-        <v>0.9938643232679153</v>
+        <v>0.9964418512943937</v>
       </c>
       <c r="F25">
-        <v>0.001520157341274223</v>
+        <v>0.001848904581266014</v>
       </c>
       <c r="G25">
-        <v>0.1106060890512307</v>
+        <v>0.08428307652786154</v>
       </c>
       <c r="H25">
-        <v>0.9594623052163809</v>
+        <v>0.9835934964510211</v>
       </c>
       <c r="I25">
-        <v>631.1598669201851</v>
+        <v>531.9871595415258</v>
       </c>
       <c r="J25">
-        <v>5475.052106713712</v>
+        <v>6208.353229103143</v>
       </c>
       <c r="K25">
-        <v>5706.375411464404</v>
+        <v>6311.909596295601</v>
       </c>
       <c r="L25">
-        <v>4.228754146039635</v>
+        <v>4.379541305876165</v>
       </c>
       <c r="M25">
-        <v>0.1093704751098669</v>
+        <v>0.1215652482450981</v>
       </c>
       <c r="N25">
-        <v>351.4540000000001</v>
+        <v>360.4100000000001</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P25">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R25">
-        <v>104.61</v>
+        <v>161.34</v>
       </c>
       <c r="S25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="U25">
-        <v>0.237347294938918</v>
+        <v>0.2214820982514571</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="300" customHeight="1">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26">
-        <v>0.6795966306215329</v>
+        <v>0.617096589656258</v>
       </c>
       <c r="E26">
-        <v>0.9925873942601608</v>
+        <v>0.9885207435490873</v>
       </c>
       <c r="F26">
-        <v>0.001154963379423137</v>
+        <v>0.001089635794508605</v>
       </c>
       <c r="G26">
-        <v>0.1215329780587316</v>
+        <v>0.1510852063345707</v>
       </c>
       <c r="H26">
-        <v>0.9289589962844592</v>
+        <v>0.9533043442585107</v>
       </c>
       <c r="I26">
-        <v>804.3190051172368</v>
+        <v>874.8834693783385</v>
       </c>
       <c r="J26">
-        <v>6147.955786331048</v>
+        <v>5520.263911421012</v>
       </c>
       <c r="K26">
-        <v>6618.113190055662</v>
+        <v>5790.662703540627</v>
       </c>
       <c r="L26">
-        <v>4.426705183873509</v>
+        <v>4.123739521244634</v>
       </c>
       <c r="M26">
-        <v>0.07879367654337684</v>
+        <v>0.157538447957813</v>
       </c>
       <c r="N26">
-        <v>373.4750000000001</v>
+        <v>370.3920000000001</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P26">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="Q26">
         <v>1</v>
       </c>
       <c r="R26">
-        <v>98.22999999999999</v>
+        <v>158.92</v>
       </c>
       <c r="S26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="T26">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U26">
-        <v>0.2339373970345964</v>
+        <v>0.2122270742358079</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="300" customHeight="1">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D27">
-        <v>0.4143800737108312</v>
+        <v>0.2860558973732849</v>
       </c>
       <c r="E27">
-        <v>0.9658702073489382</v>
+        <v>0.9357911098369885</v>
       </c>
       <c r="F27">
-        <v>0.0006543762115600864</v>
+        <v>0.0005192902116493809</v>
       </c>
       <c r="G27">
-        <v>0.2590265286717156</v>
+        <v>0.3525549584817341</v>
       </c>
       <c r="H27">
-        <v>0.8688566129982944</v>
+        <v>0.779151956548083</v>
       </c>
       <c r="I27">
-        <v>1327.763139382572</v>
+        <v>1500.417183049385</v>
       </c>
       <c r="J27">
-        <v>4453.736032613155</v>
+        <v>3315.94537443404</v>
       </c>
       <c r="K27">
-        <v>5125.973568002178</v>
+        <v>4255.83911657598</v>
       </c>
       <c r="L27">
-        <v>4.03933677084367</v>
+        <v>3.609048097763568</v>
       </c>
       <c r="M27">
-        <v>0.194150382843434</v>
+        <v>0.1911379476084967</v>
       </c>
       <c r="N27">
-        <v>353.4040000000001</v>
+        <v>373.4550000000003</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P27">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27">
-        <v>103.78</v>
+        <v>104.71</v>
       </c>
       <c r="S27">
         <v>10</v>
       </c>
       <c r="T27">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U27">
-        <v>0.232355273592387</v>
+        <v>0.2097053726169844</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="300" customHeight="1">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28">
-        <v>0.2407922799886219</v>
+        <v>0.4093797273877731</v>
       </c>
       <c r="E28">
-        <v>0.9169573768512359</v>
+        <v>0.9650801119612901</v>
       </c>
       <c r="F28">
-        <v>0.0004200203156350914</v>
+        <v>0.0007003996280037913</v>
       </c>
       <c r="G28">
-        <v>0.3989851739577555</v>
+        <v>0.2619549150078763</v>
       </c>
       <c r="H28">
-        <v>0.7249629141317616</v>
+        <v>0.8468507247238215</v>
       </c>
       <c r="I28">
-        <v>1726.018688014131</v>
+        <v>1209.096479873112</v>
       </c>
       <c r="J28">
-        <v>3136.205602569813</v>
+        <v>3908.780372419354</v>
       </c>
       <c r="K28">
-        <v>4326.022119801579</v>
+        <v>4615.666325011532</v>
       </c>
       <c r="L28">
-        <v>3.707356174106399</v>
+        <v>3.748995592736661</v>
       </c>
       <c r="M28">
-        <v>0.1806839846097422</v>
+        <v>0.1638912705248229</v>
       </c>
       <c r="N28">
-        <v>357.4360000000001</v>
+        <v>364.4110000000001</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28">
-        <v>97.63</v>
+        <v>126.35</v>
       </c>
       <c r="S28">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T28">
         <v>4</v>
       </c>
       <c r="U28">
-        <v>0.223717409587889</v>
+        <v>0.2078285181733458</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="300" customHeight="1">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29">
-        <v>0.235197908468129</v>
+        <v>0.3358296370002767</v>
       </c>
       <c r="E29">
-        <v>0.9183381964617253</v>
+        <v>0.9497828698941381</v>
       </c>
       <c r="F29">
-        <v>0.0005593956038327794</v>
+        <v>0.0005662098120762191</v>
       </c>
       <c r="G29">
-        <v>0.3957966105456509</v>
+        <v>0.3129097314812288</v>
       </c>
       <c r="H29">
-        <v>0.8364846251807048</v>
+        <v>0.7979388611541306</v>
       </c>
       <c r="I29">
-        <v>1495.336429978016</v>
+        <v>1409.263570032795</v>
       </c>
       <c r="J29">
-        <v>3160.274494076154</v>
+        <v>3593.707881231016</v>
       </c>
       <c r="K29">
-        <v>3778.042535322684</v>
+        <v>4503.73838922084</v>
       </c>
       <c r="L29">
-        <v>3.450183862249772</v>
+        <v>3.782760150370972</v>
       </c>
       <c r="M29">
-        <v>0.326678245529735</v>
+        <v>0.1504711494653002</v>
       </c>
       <c r="N29">
-        <v>373.3950000000002</v>
+        <v>353.3550000000001</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29">
+        <v>161.73</v>
+      </c>
+      <c r="S29">
         <v>10</v>
       </c>
-      <c r="Q29">
-        <v>1</v>
-      </c>
-      <c r="R29">
-        <v>153.61</v>
-      </c>
-      <c r="S29">
-        <v>13</v>
-      </c>
       <c r="T29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U29">
-        <v>0.2131147540983606</v>
+        <v>0.1594360086767896</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="300" customHeight="1">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30">
-        <v>0.5848817959131735</v>
+        <v>0.3543749643200569</v>
       </c>
       <c r="E30">
-        <v>0.9862972090738625</v>
+        <v>0.9539126084243328</v>
       </c>
       <c r="F30">
-        <v>0.0009341481804297294</v>
+        <v>0.0004694068566635343</v>
       </c>
       <c r="G30">
-        <v>0.1649782269668014</v>
+        <v>0.3000845472347508</v>
       </c>
       <c r="H30">
-        <v>0.8875386184907657</v>
+        <v>0.7897987436098777</v>
       </c>
       <c r="I30">
-        <v>950.1047447124263</v>
+        <v>1682.546244048576</v>
       </c>
       <c r="J30">
-        <v>5111.308734777933</v>
+        <v>4428.328355660146</v>
       </c>
       <c r="K30">
-        <v>5758.970514961444</v>
+        <v>5606.907318464318</v>
       </c>
       <c r="L30">
-        <v>4.192504361023125</v>
+        <v>4.078369046938212</v>
       </c>
       <c r="M30">
-        <v>0.07516633597461307</v>
+        <v>0.1320097441927729</v>
       </c>
       <c r="N30">
-        <v>360.4360000000001</v>
+        <v>373.4110000000001</v>
       </c>
       <c r="O30">
+        <v>-1</v>
+      </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
+      <c r="Q30">
         <v>0</v>
       </c>
-      <c r="P30">
-        <v>8</v>
-      </c>
-      <c r="Q30">
-        <v>2</v>
-      </c>
       <c r="R30">
-        <v>113.64</v>
+        <v>128.9</v>
       </c>
       <c r="S30">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U30">
-        <v>0.2097053726169844</v>
+        <v>0.1492693110647182</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="300" customHeight="1">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D31">
-        <v>0.2813297056408623</v>
+        <v>0.3087218118031491</v>
       </c>
       <c r="E31">
-        <v>0.9327933965186915</v>
+        <v>0.9426428158079821</v>
       </c>
       <c r="F31">
-        <v>0.0005124871549688345</v>
+        <v>0.0007446449785900767</v>
       </c>
       <c r="G31">
-        <v>0.3604115417285124</v>
+        <v>0.3338031183281526</v>
       </c>
       <c r="H31">
-        <v>0.7405292505034669</v>
+        <v>0.8797732561958111</v>
       </c>
       <c r="I31">
-        <v>1444.971338937266</v>
+        <v>1181.466714328201</v>
       </c>
       <c r="J31">
-        <v>2968.949155985236</v>
+        <v>3113.879892906392</v>
       </c>
       <c r="K31">
-        <v>4009.226042005395</v>
+        <v>3539.411855244365</v>
       </c>
       <c r="L31">
-        <v>3.549668295417375</v>
+        <v>3.373492571096413</v>
       </c>
       <c r="M31">
-        <v>0.1500774932676833</v>
+        <v>0.2395740830217949</v>
       </c>
       <c r="N31">
-        <v>361.4640000000001</v>
+        <v>356.3160000000001</v>
       </c>
       <c r="O31">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P31">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q31">
         <v>0</v>
       </c>
       <c r="R31">
-        <v>87.22999999999999</v>
+        <v>151.19</v>
       </c>
       <c r="S31">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="T31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="U31">
-        <v>0.2081563296516568</v>
+        <v>0.1365422396856582</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="300" customHeight="1">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D32">
-        <v>0.360393832452292</v>
+        <v>0.2346434074751484</v>
       </c>
       <c r="E32">
-        <v>0.9551647918592746</v>
+        <v>0.9148691580678614</v>
       </c>
       <c r="F32">
-        <v>0.0008743382020202426</v>
+        <v>0.000398744731877335</v>
       </c>
       <c r="G32">
-        <v>0.2960746871862378</v>
+        <v>0.40375044720248</v>
       </c>
       <c r="H32">
-        <v>0.8942044442696888</v>
+        <v>0.7318177409164538</v>
       </c>
       <c r="I32">
-        <v>1022.721462019552</v>
+        <v>1835.303848331672</v>
       </c>
       <c r="J32">
-        <v>3088.822233602907</v>
+        <v>3326.579389540076</v>
       </c>
       <c r="K32">
-        <v>3454.268487924591</v>
+        <v>4545.639171543187</v>
       </c>
       <c r="L32">
-        <v>3.354023763081078</v>
+        <v>3.722648155628957</v>
       </c>
       <c r="M32">
-        <v>0.2774593735321926</v>
+        <v>0.1943125815895837</v>
       </c>
       <c r="N32">
-        <v>350.3860000000001</v>
+        <v>368.3910000000001</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P32">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q32">
         <v>0</v>
       </c>
       <c r="R32">
-        <v>155.48</v>
+        <v>119.94</v>
       </c>
       <c r="S32">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="T32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U32">
-        <v>0.186536901865369</v>
+        <v>0.09040178571428571</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="300" customHeight="1">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33">
-        <v>0.4390340502597004</v>
+        <v>0.6174353324483948</v>
       </c>
       <c r="E33">
-        <v>0.9695900877354237</v>
+        <v>0.9887717285503071</v>
       </c>
       <c r="F33">
-        <v>0.0008423005632410761</v>
+        <v>0.0009903215224338997</v>
       </c>
       <c r="G33">
-        <v>0.2447346762623012</v>
+        <v>0.1494338275613584</v>
       </c>
       <c r="H33">
-        <v>0.8997335592361099</v>
+        <v>0.8946424796103746</v>
       </c>
       <c r="I33">
-        <v>1068.185869155825</v>
+        <v>903.3858795794157</v>
       </c>
       <c r="J33">
-        <v>3927.039227376266</v>
+        <v>5408.463375001708</v>
       </c>
       <c r="K33">
-        <v>4364.669059038315</v>
+        <v>6045.390754703652</v>
       </c>
       <c r="L33">
-        <v>3.799197437509039</v>
+        <v>4.152644592290833</v>
       </c>
       <c r="M33">
-        <v>0.2158601450336576</v>
+        <v>0.05802703412181837</v>
       </c>
       <c r="N33">
-        <v>350.4410000000002</v>
+        <v>369.3840000000001</v>
       </c>
       <c r="O33">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="P33">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R33">
-        <v>116.41</v>
+        <v>157.3</v>
       </c>
       <c r="S33">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T33">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U33">
-        <v>0.1787487586891758</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="300" customHeight="1">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34">
-        <v>0.7192041818456747</v>
-      </c>
-      <c r="E34">
-        <v>0.9944885824345713</v>
-      </c>
-      <c r="F34">
-        <v>0.001451229349131963</v>
-      </c>
-      <c r="G34">
-        <v>0.1048449302888662</v>
-      </c>
-      <c r="H34">
-        <v>0.9524863662367077</v>
-      </c>
-      <c r="I34">
-        <v>656.3306942534116</v>
-      </c>
-      <c r="J34">
-        <v>5962.577649645631</v>
-      </c>
-      <c r="K34">
-        <v>6260.013645343704</v>
-      </c>
-      <c r="L34">
-        <v>4.376203274249526</v>
-      </c>
-      <c r="M34">
-        <v>0.08898260413669914</v>
-      </c>
-      <c r="N34">
-        <v>352.3720000000001</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>6</v>
-      </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>107.96</v>
-      </c>
-      <c r="S34">
-        <v>10</v>
-      </c>
-      <c r="T34">
-        <v>3</v>
-      </c>
-      <c r="U34">
-        <v>0.1492693110647182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="300" customHeight="1">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35">
-        <v>0.5207746956644161</v>
-      </c>
-      <c r="E35">
-        <v>0.9802838849018404</v>
-      </c>
-      <c r="F35">
-        <v>0.0008912360400703853</v>
-      </c>
-      <c r="G35">
-        <v>0.1975942939503953</v>
-      </c>
-      <c r="H35">
-        <v>0.8800692462864887</v>
-      </c>
-      <c r="I35">
-        <v>987.4704418562173</v>
-      </c>
-      <c r="J35">
-        <v>4398.114693093084</v>
-      </c>
-      <c r="K35">
-        <v>4997.46436050484</v>
-      </c>
-      <c r="L35">
-        <v>3.883289484747549</v>
-      </c>
-      <c r="M35">
-        <v>0.104936010932161</v>
-      </c>
-      <c r="N35">
-        <v>372.491</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>6</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>81.24000000000001</v>
-      </c>
-      <c r="S35">
-        <v>9</v>
-      </c>
-      <c r="T35">
-        <v>5</v>
-      </c>
-      <c r="U35">
-        <v>0.1444788441692466</v>
+        <v>0.07623888182973317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>